<commit_message>
Ajout Footer aux pages
</commit_message>
<xml_diff>
--- a/Documentation/RodriguesF_TPI_Planning.xlsx
+++ b/Documentation/RodriguesF_TPI_Planning.xlsx
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="60">
   <si>
     <t>Listes des tâches</t>
   </si>
@@ -16768,11 +16768,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:EQ84"/>
+  <dimension ref="A1:EQ82"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B38" sqref="B38"/>
+      <pane ySplit="2" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21981,8 +21981,8 @@
         <v>22</v>
       </c>
       <c r="C34" s="9">
-        <f t="shared" ref="C34:C41" si="3">IF($B34&gt;"",SUM(COUNTIF($D34:$EQ34,"R")),"")</f>
-        <v>1</v>
+        <f t="shared" ref="C34:C39" si="3">IF($B34&gt;"",SUM(COUNTIF($D34:$EQ34,"R")),"")</f>
+        <v>2</v>
       </c>
       <c r="D34" s="34"/>
       <c r="E34" s="35"/>
@@ -21992,7 +21992,9 @@
       <c r="I34" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="J34" s="35"/>
+      <c r="J34" s="35" t="s">
+        <v>58</v>
+      </c>
       <c r="K34" s="35"/>
       <c r="L34" s="34"/>
       <c r="M34" s="44"/>
@@ -22138,15 +22140,19 @@
       </c>
       <c r="C35" s="9">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D35" s="34"/>
       <c r="E35" s="35"/>
       <c r="F35" s="35"/>
       <c r="G35" s="35"/>
       <c r="H35" s="35"/>
-      <c r="I35" s="35"/>
-      <c r="J35" s="35"/>
+      <c r="I35" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="J35" s="35" t="s">
+        <v>58</v>
+      </c>
       <c r="K35" s="35"/>
       <c r="L35" s="34"/>
       <c r="M35" s="44"/>
@@ -22292,15 +22298,19 @@
       </c>
       <c r="C36" s="9">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D36" s="34"/>
       <c r="E36" s="35"/>
       <c r="F36" s="35"/>
       <c r="G36" s="35"/>
       <c r="H36" s="35"/>
-      <c r="I36" s="35"/>
-      <c r="J36" s="35"/>
+      <c r="I36" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="J36" s="35" t="s">
+        <v>58</v>
+      </c>
       <c r="K36" s="35"/>
       <c r="L36" s="34"/>
       <c r="M36" s="44"/>
@@ -22450,8 +22460,12 @@
       <c r="F37" s="35"/>
       <c r="G37" s="35"/>
       <c r="H37" s="35"/>
-      <c r="I37" s="35"/>
-      <c r="J37" s="35"/>
+      <c r="I37" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="J37" s="35" t="s">
+        <v>58</v>
+      </c>
       <c r="K37" s="35"/>
       <c r="L37" s="34"/>
       <c r="M37" s="44"/>
@@ -22593,19 +22607,23 @@
     <row r="38" spans="1:147" x14ac:dyDescent="0.25">
       <c r="A38" s="21"/>
       <c r="B38" s="55" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C38" s="9">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D38" s="34"/>
       <c r="E38" s="35"/>
       <c r="F38" s="35"/>
       <c r="G38" s="35"/>
       <c r="H38" s="35"/>
-      <c r="I38" s="35"/>
-      <c r="J38" s="35"/>
+      <c r="I38" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="J38" s="35" t="s">
+        <v>58</v>
+      </c>
       <c r="K38" s="35"/>
       <c r="L38" s="34"/>
       <c r="M38" s="44"/>
@@ -22745,21 +22763,25 @@
       <c r="EQ38" s="72"/>
     </row>
     <row r="39" spans="1:147" x14ac:dyDescent="0.25">
-      <c r="A39" s="16"/>
+      <c r="A39" s="21"/>
       <c r="B39" s="55" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C39" s="9">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D39" s="34"/>
       <c r="E39" s="35"/>
       <c r="F39" s="35"/>
       <c r="G39" s="35"/>
       <c r="H39" s="35"/>
-      <c r="I39" s="35"/>
-      <c r="J39" s="35"/>
+      <c r="I39" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="J39" s="35" t="s">
+        <v>58</v>
+      </c>
       <c r="K39" s="35"/>
       <c r="L39" s="34"/>
       <c r="M39" s="44"/>
@@ -22901,19 +22923,20 @@
     <row r="40" spans="1:147" x14ac:dyDescent="0.25">
       <c r="A40" s="21"/>
       <c r="B40" s="55" t="s">
-        <v>27</v>
-      </c>
-      <c r="C40" s="9">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="C40" s="9"/>
       <c r="D40" s="34"/>
       <c r="E40" s="35"/>
       <c r="F40" s="35"/>
       <c r="G40" s="35"/>
       <c r="H40" s="35"/>
-      <c r="I40" s="35"/>
-      <c r="J40" s="35"/>
+      <c r="I40" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="J40" s="35" t="s">
+        <v>58</v>
+      </c>
       <c r="K40" s="35"/>
       <c r="L40" s="34"/>
       <c r="M40" s="44"/>
@@ -23052,13 +23075,13 @@
       <c r="EP40" s="44"/>
       <c r="EQ40" s="72"/>
     </row>
-    <row r="41" spans="1:147" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:147" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="21"/>
       <c r="B41" s="55" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C41" s="9">
-        <f t="shared" si="3"/>
+        <f>IF($B41&gt;"",SUM(COUNTIF($D41:$EQ41,"R")),"")</f>
         <v>0</v>
       </c>
       <c r="D41" s="34"/>
@@ -23209,9 +23232,12 @@
     <row r="42" spans="1:147" x14ac:dyDescent="0.25">
       <c r="A42" s="21"/>
       <c r="B42" s="55" t="s">
-        <v>42</v>
-      </c>
-      <c r="C42" s="9"/>
+        <v>30</v>
+      </c>
+      <c r="C42" s="9">
+        <f>IF($B42&gt;"",SUM(COUNTIF($D42:$EQ42,"R")),"")</f>
+        <v>0</v>
+      </c>
       <c r="D42" s="34"/>
       <c r="E42" s="35"/>
       <c r="F42" s="35"/>
@@ -23357,10 +23383,10 @@
       <c r="EP42" s="44"/>
       <c r="EQ42" s="72"/>
     </row>
-    <row r="43" spans="1:147" ht="30" x14ac:dyDescent="0.25">
-      <c r="A43" s="21"/>
+    <row r="43" spans="1:147" x14ac:dyDescent="0.25">
+      <c r="A43" s="16"/>
       <c r="B43" s="55" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C43" s="9">
         <f>IF($B43&gt;"",SUM(COUNTIF($D43:$EQ43,"R")),"")</f>
@@ -23512,46 +23538,46 @@
       <c r="EQ43" s="72"/>
     </row>
     <row r="44" spans="1:147" x14ac:dyDescent="0.25">
-      <c r="A44" s="21"/>
-      <c r="B44" s="55" t="s">
-        <v>30</v>
+      <c r="A44" s="64"/>
+      <c r="B44" s="65" t="s">
+        <v>33</v>
       </c>
       <c r="C44" s="9">
         <f>IF($B44&gt;"",SUM(COUNTIF($D44:$EQ44,"R")),"")</f>
         <v>0</v>
       </c>
-      <c r="D44" s="34"/>
-      <c r="E44" s="35"/>
-      <c r="F44" s="35"/>
-      <c r="G44" s="35"/>
-      <c r="H44" s="35"/>
-      <c r="I44" s="35"/>
-      <c r="J44" s="35"/>
-      <c r="K44" s="35"/>
-      <c r="L44" s="34"/>
-      <c r="M44" s="44"/>
-      <c r="N44" s="44"/>
-      <c r="O44" s="44"/>
-      <c r="P44" s="44"/>
-      <c r="Q44" s="44"/>
-      <c r="R44" s="44"/>
-      <c r="S44" s="44"/>
-      <c r="T44" s="34"/>
-      <c r="U44" s="44"/>
-      <c r="V44" s="44"/>
-      <c r="W44" s="44"/>
-      <c r="X44" s="44"/>
-      <c r="Y44" s="44"/>
-      <c r="Z44" s="44"/>
-      <c r="AA44" s="44"/>
-      <c r="AB44" s="34"/>
-      <c r="AC44" s="44"/>
-      <c r="AD44" s="44"/>
-      <c r="AE44" s="44"/>
-      <c r="AF44" s="44"/>
-      <c r="AG44" s="44"/>
-      <c r="AH44" s="44"/>
-      <c r="AI44" s="44"/>
+      <c r="D44" s="66"/>
+      <c r="E44" s="67"/>
+      <c r="F44" s="67"/>
+      <c r="G44" s="67"/>
+      <c r="H44" s="67"/>
+      <c r="I44" s="67"/>
+      <c r="J44" s="67"/>
+      <c r="K44" s="67"/>
+      <c r="L44" s="66"/>
+      <c r="M44" s="68"/>
+      <c r="N44" s="68"/>
+      <c r="O44" s="68"/>
+      <c r="P44" s="68"/>
+      <c r="Q44" s="68"/>
+      <c r="R44" s="68"/>
+      <c r="S44" s="68"/>
+      <c r="T44" s="66"/>
+      <c r="U44" s="68"/>
+      <c r="V44" s="68"/>
+      <c r="W44" s="68"/>
+      <c r="X44" s="68"/>
+      <c r="Y44" s="68"/>
+      <c r="Z44" s="68"/>
+      <c r="AA44" s="68"/>
+      <c r="AB44" s="66"/>
+      <c r="AC44" s="68"/>
+      <c r="AD44" s="68"/>
+      <c r="AE44" s="68"/>
+      <c r="AF44" s="68"/>
+      <c r="AG44" s="68"/>
+      <c r="AH44" s="68"/>
+      <c r="AI44" s="68"/>
       <c r="AJ44" s="86"/>
       <c r="AK44" s="87"/>
       <c r="AL44" s="87"/>
@@ -23576,30 +23602,30 @@
       <c r="BE44" s="87"/>
       <c r="BF44" s="87"/>
       <c r="BG44" s="87"/>
-      <c r="BH44" s="34"/>
-      <c r="BI44" s="35"/>
-      <c r="BJ44" s="35"/>
-      <c r="BK44" s="35"/>
-      <c r="BL44" s="35"/>
-      <c r="BM44" s="35"/>
-      <c r="BN44" s="35"/>
-      <c r="BO44" s="35"/>
-      <c r="BP44" s="34"/>
-      <c r="BQ44" s="44"/>
-      <c r="BR44" s="44"/>
-      <c r="BS44" s="44"/>
-      <c r="BT44" s="44"/>
-      <c r="BU44" s="44"/>
-      <c r="BV44" s="44"/>
-      <c r="BW44" s="44"/>
-      <c r="BX44" s="34"/>
-      <c r="BY44" s="44"/>
-      <c r="BZ44" s="44"/>
-      <c r="CA44" s="44"/>
-      <c r="CB44" s="44"/>
-      <c r="CC44" s="44"/>
-      <c r="CD44" s="44"/>
-      <c r="CE44" s="44"/>
+      <c r="BH44" s="66"/>
+      <c r="BI44" s="67"/>
+      <c r="BJ44" s="67"/>
+      <c r="BK44" s="67"/>
+      <c r="BL44" s="67"/>
+      <c r="BM44" s="67"/>
+      <c r="BN44" s="67"/>
+      <c r="BO44" s="67"/>
+      <c r="BP44" s="66"/>
+      <c r="BQ44" s="68"/>
+      <c r="BR44" s="68"/>
+      <c r="BS44" s="68"/>
+      <c r="BT44" s="68"/>
+      <c r="BU44" s="68"/>
+      <c r="BV44" s="68"/>
+      <c r="BW44" s="68"/>
+      <c r="BX44" s="66"/>
+      <c r="BY44" s="68"/>
+      <c r="BZ44" s="68"/>
+      <c r="CA44" s="68"/>
+      <c r="CB44" s="68"/>
+      <c r="CC44" s="68"/>
+      <c r="CD44" s="68"/>
+      <c r="CE44" s="68"/>
       <c r="CF44" s="86"/>
       <c r="CG44" s="87"/>
       <c r="CH44" s="87"/>
@@ -23632,80 +23658,80 @@
       <c r="DI44" s="87"/>
       <c r="DJ44" s="87"/>
       <c r="DK44" s="87"/>
-      <c r="DL44" s="34"/>
-      <c r="DM44" s="44"/>
-      <c r="DN44" s="44"/>
-      <c r="DO44" s="44"/>
-      <c r="DP44" s="44"/>
-      <c r="DQ44" s="44"/>
-      <c r="DR44" s="44"/>
-      <c r="DS44" s="44"/>
-      <c r="DT44" s="34"/>
-      <c r="DU44" s="44"/>
-      <c r="DV44" s="44"/>
-      <c r="DW44" s="44"/>
-      <c r="DX44" s="44"/>
-      <c r="DY44" s="44"/>
-      <c r="DZ44" s="44"/>
-      <c r="EA44" s="44"/>
-      <c r="EB44" s="34"/>
-      <c r="EC44" s="35"/>
-      <c r="ED44" s="44"/>
-      <c r="EE44" s="44"/>
-      <c r="EF44" s="44"/>
-      <c r="EG44" s="44"/>
-      <c r="EH44" s="44"/>
-      <c r="EI44" s="44"/>
-      <c r="EJ44" s="34"/>
-      <c r="EK44" s="35"/>
-      <c r="EL44" s="44"/>
-      <c r="EM44" s="44"/>
-      <c r="EN44" s="44"/>
-      <c r="EO44" s="44"/>
-      <c r="EP44" s="44"/>
-      <c r="EQ44" s="72"/>
+      <c r="DL44" s="66"/>
+      <c r="DM44" s="68"/>
+      <c r="DN44" s="68"/>
+      <c r="DO44" s="68"/>
+      <c r="DP44" s="68"/>
+      <c r="DQ44" s="68"/>
+      <c r="DR44" s="68"/>
+      <c r="DS44" s="68"/>
+      <c r="DT44" s="66"/>
+      <c r="DU44" s="68"/>
+      <c r="DV44" s="68"/>
+      <c r="DW44" s="68"/>
+      <c r="DX44" s="68"/>
+      <c r="DY44" s="68"/>
+      <c r="DZ44" s="68"/>
+      <c r="EA44" s="68"/>
+      <c r="EB44" s="66"/>
+      <c r="EC44" s="67"/>
+      <c r="ED44" s="68"/>
+      <c r="EE44" s="68"/>
+      <c r="EF44" s="68"/>
+      <c r="EG44" s="68"/>
+      <c r="EH44" s="68"/>
+      <c r="EI44" s="68"/>
+      <c r="EJ44" s="66"/>
+      <c r="EK44" s="67"/>
+      <c r="EL44" s="68"/>
+      <c r="EM44" s="68"/>
+      <c r="EN44" s="68"/>
+      <c r="EO44" s="68"/>
+      <c r="EP44" s="68"/>
+      <c r="EQ44" s="74"/>
     </row>
     <row r="45" spans="1:147" x14ac:dyDescent="0.25">
-      <c r="A45" s="16"/>
-      <c r="B45" s="55" t="s">
-        <v>31</v>
+      <c r="A45" s="64"/>
+      <c r="B45" s="65" t="s">
+        <v>32</v>
       </c>
       <c r="C45" s="9">
         <f>IF($B45&gt;"",SUM(COUNTIF($D45:$EQ45,"R")),"")</f>
         <v>0</v>
       </c>
-      <c r="D45" s="34"/>
-      <c r="E45" s="35"/>
-      <c r="F45" s="35"/>
-      <c r="G45" s="35"/>
-      <c r="H45" s="35"/>
-      <c r="I45" s="35"/>
-      <c r="J45" s="35"/>
-      <c r="K45" s="35"/>
-      <c r="L45" s="34"/>
-      <c r="M45" s="44"/>
-      <c r="N45" s="44"/>
-      <c r="O45" s="44"/>
-      <c r="P45" s="44"/>
-      <c r="Q45" s="44"/>
-      <c r="R45" s="44"/>
-      <c r="S45" s="44"/>
-      <c r="T45" s="34"/>
-      <c r="U45" s="44"/>
-      <c r="V45" s="44"/>
-      <c r="W45" s="44"/>
-      <c r="X45" s="44"/>
-      <c r="Y45" s="44"/>
-      <c r="Z45" s="44"/>
-      <c r="AA45" s="44"/>
-      <c r="AB45" s="34"/>
-      <c r="AC45" s="44"/>
-      <c r="AD45" s="44"/>
-      <c r="AE45" s="44"/>
-      <c r="AF45" s="44"/>
-      <c r="AG45" s="44"/>
-      <c r="AH45" s="44"/>
-      <c r="AI45" s="44"/>
+      <c r="D45" s="66"/>
+      <c r="E45" s="67"/>
+      <c r="F45" s="67"/>
+      <c r="G45" s="67"/>
+      <c r="H45" s="67"/>
+      <c r="I45" s="67"/>
+      <c r="J45" s="67"/>
+      <c r="K45" s="67"/>
+      <c r="L45" s="66"/>
+      <c r="M45" s="68"/>
+      <c r="N45" s="68"/>
+      <c r="O45" s="68"/>
+      <c r="P45" s="68"/>
+      <c r="Q45" s="68"/>
+      <c r="R45" s="68"/>
+      <c r="S45" s="68"/>
+      <c r="T45" s="66"/>
+      <c r="U45" s="68"/>
+      <c r="V45" s="68"/>
+      <c r="W45" s="68"/>
+      <c r="X45" s="68"/>
+      <c r="Y45" s="68"/>
+      <c r="Z45" s="68"/>
+      <c r="AA45" s="68"/>
+      <c r="AB45" s="66"/>
+      <c r="AC45" s="68"/>
+      <c r="AD45" s="68"/>
+      <c r="AE45" s="68"/>
+      <c r="AF45" s="68"/>
+      <c r="AG45" s="68"/>
+      <c r="AH45" s="68"/>
+      <c r="AI45" s="68"/>
       <c r="AJ45" s="86"/>
       <c r="AK45" s="87"/>
       <c r="AL45" s="87"/>
@@ -23730,30 +23756,30 @@
       <c r="BE45" s="87"/>
       <c r="BF45" s="87"/>
       <c r="BG45" s="87"/>
-      <c r="BH45" s="34"/>
-      <c r="BI45" s="35"/>
-      <c r="BJ45" s="35"/>
-      <c r="BK45" s="35"/>
-      <c r="BL45" s="35"/>
-      <c r="BM45" s="35"/>
-      <c r="BN45" s="35"/>
-      <c r="BO45" s="35"/>
-      <c r="BP45" s="34"/>
-      <c r="BQ45" s="44"/>
-      <c r="BR45" s="44"/>
-      <c r="BS45" s="44"/>
-      <c r="BT45" s="44"/>
-      <c r="BU45" s="44"/>
-      <c r="BV45" s="44"/>
-      <c r="BW45" s="44"/>
-      <c r="BX45" s="34"/>
-      <c r="BY45" s="44"/>
-      <c r="BZ45" s="44"/>
-      <c r="CA45" s="44"/>
-      <c r="CB45" s="44"/>
-      <c r="CC45" s="44"/>
-      <c r="CD45" s="44"/>
-      <c r="CE45" s="44"/>
+      <c r="BH45" s="66"/>
+      <c r="BI45" s="67"/>
+      <c r="BJ45" s="67"/>
+      <c r="BK45" s="67"/>
+      <c r="BL45" s="67"/>
+      <c r="BM45" s="67"/>
+      <c r="BN45" s="67"/>
+      <c r="BO45" s="67"/>
+      <c r="BP45" s="66"/>
+      <c r="BQ45" s="68"/>
+      <c r="BR45" s="68"/>
+      <c r="BS45" s="68"/>
+      <c r="BT45" s="68"/>
+      <c r="BU45" s="68"/>
+      <c r="BV45" s="68"/>
+      <c r="BW45" s="68"/>
+      <c r="BX45" s="66"/>
+      <c r="BY45" s="68"/>
+      <c r="BZ45" s="68"/>
+      <c r="CA45" s="68"/>
+      <c r="CB45" s="68"/>
+      <c r="CC45" s="68"/>
+      <c r="CD45" s="68"/>
+      <c r="CE45" s="68"/>
       <c r="CF45" s="86"/>
       <c r="CG45" s="87"/>
       <c r="CH45" s="87"/>
@@ -23786,48 +23812,45 @@
       <c r="DI45" s="87"/>
       <c r="DJ45" s="87"/>
       <c r="DK45" s="87"/>
-      <c r="DL45" s="34"/>
-      <c r="DM45" s="44"/>
-      <c r="DN45" s="44"/>
-      <c r="DO45" s="44"/>
-      <c r="DP45" s="44"/>
-      <c r="DQ45" s="44"/>
-      <c r="DR45" s="44"/>
-      <c r="DS45" s="44"/>
-      <c r="DT45" s="34"/>
-      <c r="DU45" s="44"/>
-      <c r="DV45" s="44"/>
-      <c r="DW45" s="44"/>
-      <c r="DX45" s="44"/>
-      <c r="DY45" s="44"/>
-      <c r="DZ45" s="44"/>
-      <c r="EA45" s="44"/>
-      <c r="EB45" s="34"/>
-      <c r="EC45" s="35"/>
-      <c r="ED45" s="44"/>
-      <c r="EE45" s="44"/>
-      <c r="EF45" s="44"/>
-      <c r="EG45" s="44"/>
-      <c r="EH45" s="44"/>
-      <c r="EI45" s="44"/>
-      <c r="EJ45" s="34"/>
-      <c r="EK45" s="35"/>
-      <c r="EL45" s="44"/>
-      <c r="EM45" s="44"/>
-      <c r="EN45" s="44"/>
-      <c r="EO45" s="44"/>
-      <c r="EP45" s="44"/>
-      <c r="EQ45" s="72"/>
+      <c r="DL45" s="66"/>
+      <c r="DM45" s="68"/>
+      <c r="DN45" s="68"/>
+      <c r="DO45" s="68"/>
+      <c r="DP45" s="68"/>
+      <c r="DQ45" s="68"/>
+      <c r="DR45" s="68"/>
+      <c r="DS45" s="68"/>
+      <c r="DT45" s="66"/>
+      <c r="DU45" s="68"/>
+      <c r="DV45" s="68"/>
+      <c r="DW45" s="68"/>
+      <c r="DX45" s="68"/>
+      <c r="DY45" s="68"/>
+      <c r="DZ45" s="68"/>
+      <c r="EA45" s="68"/>
+      <c r="EB45" s="66"/>
+      <c r="EC45" s="67"/>
+      <c r="ED45" s="68"/>
+      <c r="EE45" s="68"/>
+      <c r="EF45" s="68"/>
+      <c r="EG45" s="68"/>
+      <c r="EH45" s="68"/>
+      <c r="EI45" s="68"/>
+      <c r="EJ45" s="66"/>
+      <c r="EK45" s="67"/>
+      <c r="EL45" s="68"/>
+      <c r="EM45" s="68"/>
+      <c r="EN45" s="68"/>
+      <c r="EO45" s="68"/>
+      <c r="EP45" s="68"/>
+      <c r="EQ45" s="74"/>
     </row>
     <row r="46" spans="1:147" x14ac:dyDescent="0.25">
       <c r="A46" s="64"/>
       <c r="B46" s="65" t="s">
-        <v>33</v>
-      </c>
-      <c r="C46" s="9">
-        <f>IF($B46&gt;"",SUM(COUNTIF($D46:$EQ46,"R")),"")</f>
-        <v>0</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="C46" s="9"/>
       <c r="D46" s="66"/>
       <c r="E46" s="67"/>
       <c r="F46" s="67"/>
@@ -23973,15 +23996,12 @@
       <c r="EP46" s="68"/>
       <c r="EQ46" s="74"/>
     </row>
-    <row r="47" spans="1:147" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:147" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="64"/>
       <c r="B47" s="65" t="s">
-        <v>32</v>
-      </c>
-      <c r="C47" s="9">
-        <f>IF($B47&gt;"",SUM(COUNTIF($D47:$EQ47,"R")),"")</f>
-        <v>0</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="C47" s="9"/>
       <c r="D47" s="66"/>
       <c r="E47" s="67"/>
       <c r="F47" s="67"/>
@@ -24127,12 +24147,15 @@
       <c r="EP47" s="68"/>
       <c r="EQ47" s="74"/>
     </row>
-    <row r="48" spans="1:147" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:147" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="64"/>
       <c r="B48" s="65" t="s">
-        <v>44</v>
-      </c>
-      <c r="C48" s="9"/>
+        <v>38</v>
+      </c>
+      <c r="C48" s="9">
+        <f t="shared" ref="C48:C55" si="4">IF($B48&gt;"",SUM(COUNTIF($D48:$EQ48,"R")),"")</f>
+        <v>0</v>
+      </c>
       <c r="D48" s="66"/>
       <c r="E48" s="67"/>
       <c r="F48" s="67"/>
@@ -24278,12 +24301,15 @@
       <c r="EP48" s="68"/>
       <c r="EQ48" s="74"/>
     </row>
-    <row r="49" spans="1:147" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:147" x14ac:dyDescent="0.25">
       <c r="A49" s="64"/>
       <c r="B49" s="65" t="s">
-        <v>55</v>
-      </c>
-      <c r="C49" s="9"/>
+        <v>34</v>
+      </c>
+      <c r="C49" s="9">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
       <c r="D49" s="66"/>
       <c r="E49" s="67"/>
       <c r="F49" s="67"/>
@@ -24429,13 +24455,13 @@
       <c r="EP49" s="68"/>
       <c r="EQ49" s="74"/>
     </row>
-    <row r="50" spans="1:147" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:147" x14ac:dyDescent="0.25">
       <c r="A50" s="64"/>
       <c r="B50" s="65" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C50" s="9">
-        <f t="shared" ref="C50:C57" si="4">IF($B50&gt;"",SUM(COUNTIF($D50:$EQ50,"R")),"")</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="D50" s="66"/>
@@ -24583,10 +24609,10 @@
       <c r="EP50" s="68"/>
       <c r="EQ50" s="74"/>
     </row>
-    <row r="51" spans="1:147" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:147" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="64"/>
       <c r="B51" s="65" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C51" s="9">
         <f t="shared" si="4"/>
@@ -24740,7 +24766,7 @@
     <row r="52" spans="1:147" x14ac:dyDescent="0.25">
       <c r="A52" s="64"/>
       <c r="B52" s="65" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="C52" s="9">
         <f t="shared" si="4"/>
@@ -24894,7 +24920,7 @@
     <row r="53" spans="1:147" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="64"/>
       <c r="B53" s="65" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="C53" s="9">
         <f t="shared" si="4"/>
@@ -25045,12 +25071,12 @@
       <c r="EP53" s="68"/>
       <c r="EQ53" s="74"/>
     </row>
-    <row r="54" spans="1:147" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:147" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="64"/>
       <c r="B54" s="65" t="s">
-        <v>51</v>
-      </c>
-      <c r="C54" s="9">
+        <v>37</v>
+      </c>
+      <c r="C54" s="48">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -25202,9 +25228,9 @@
     <row r="55" spans="1:147" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="64"/>
       <c r="B55" s="65" t="s">
-        <v>54</v>
-      </c>
-      <c r="C55" s="9">
+        <v>43</v>
+      </c>
+      <c r="C55" s="48">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -25353,15 +25379,10 @@
       <c r="EP55" s="68"/>
       <c r="EQ55" s="74"/>
     </row>
-    <row r="56" spans="1:147" ht="30" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:147" x14ac:dyDescent="0.25">
       <c r="A56" s="64"/>
-      <c r="B56" s="65" t="s">
-        <v>37</v>
-      </c>
-      <c r="C56" s="48">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
+      <c r="B56" s="65"/>
+      <c r="C56" s="48"/>
       <c r="D56" s="66"/>
       <c r="E56" s="67"/>
       <c r="F56" s="67"/>
@@ -25507,15 +25528,10 @@
       <c r="EP56" s="68"/>
       <c r="EQ56" s="74"/>
     </row>
-    <row r="57" spans="1:147" ht="30" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:147" x14ac:dyDescent="0.25">
       <c r="A57" s="64"/>
-      <c r="B57" s="65" t="s">
-        <v>43</v>
-      </c>
-      <c r="C57" s="48">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
+      <c r="B57" s="65"/>
+      <c r="C57" s="48"/>
       <c r="D57" s="66"/>
       <c r="E57" s="67"/>
       <c r="F57" s="67"/>
@@ -25810,42 +25826,45 @@
       <c r="EP58" s="68"/>
       <c r="EQ58" s="74"/>
     </row>
-    <row r="59" spans="1:147" x14ac:dyDescent="0.25">
-      <c r="A59" s="64"/>
-      <c r="B59" s="65"/>
-      <c r="C59" s="48"/>
-      <c r="D59" s="66"/>
-      <c r="E59" s="67"/>
-      <c r="F59" s="67"/>
-      <c r="G59" s="67"/>
-      <c r="H59" s="67"/>
-      <c r="I59" s="67"/>
-      <c r="J59" s="67"/>
-      <c r="K59" s="67"/>
-      <c r="L59" s="66"/>
-      <c r="M59" s="68"/>
-      <c r="N59" s="68"/>
-      <c r="O59" s="68"/>
-      <c r="P59" s="68"/>
-      <c r="Q59" s="68"/>
-      <c r="R59" s="68"/>
-      <c r="S59" s="68"/>
-      <c r="T59" s="66"/>
-      <c r="U59" s="68"/>
-      <c r="V59" s="68"/>
-      <c r="W59" s="68"/>
-      <c r="X59" s="68"/>
-      <c r="Y59" s="68"/>
-      <c r="Z59" s="68"/>
-      <c r="AA59" s="68"/>
-      <c r="AB59" s="66"/>
-      <c r="AC59" s="68"/>
-      <c r="AD59" s="68"/>
-      <c r="AE59" s="68"/>
-      <c r="AF59" s="68"/>
-      <c r="AG59" s="68"/>
-      <c r="AH59" s="68"/>
-      <c r="AI59" s="68"/>
+    <row r="59" spans="1:147" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="17"/>
+      <c r="B59" s="60"/>
+      <c r="C59" s="50" t="str">
+        <f>IF($B59&gt;"",SUM(COUNTIF($D59:$EQ59,"R")),"")</f>
+        <v/>
+      </c>
+      <c r="D59" s="36"/>
+      <c r="E59" s="37"/>
+      <c r="F59" s="37"/>
+      <c r="G59" s="37"/>
+      <c r="H59" s="37"/>
+      <c r="I59" s="37"/>
+      <c r="J59" s="37"/>
+      <c r="K59" s="37"/>
+      <c r="L59" s="36"/>
+      <c r="M59" s="45"/>
+      <c r="N59" s="45"/>
+      <c r="O59" s="45"/>
+      <c r="P59" s="45"/>
+      <c r="Q59" s="45"/>
+      <c r="R59" s="45"/>
+      <c r="S59" s="45"/>
+      <c r="T59" s="36"/>
+      <c r="U59" s="45"/>
+      <c r="V59" s="45"/>
+      <c r="W59" s="45"/>
+      <c r="X59" s="45"/>
+      <c r="Y59" s="45"/>
+      <c r="Z59" s="45"/>
+      <c r="AA59" s="45"/>
+      <c r="AB59" s="36"/>
+      <c r="AC59" s="45"/>
+      <c r="AD59" s="45"/>
+      <c r="AE59" s="45"/>
+      <c r="AF59" s="45"/>
+      <c r="AG59" s="45"/>
+      <c r="AH59" s="45"/>
+      <c r="AI59" s="45"/>
       <c r="AJ59" s="86"/>
       <c r="AK59" s="87"/>
       <c r="AL59" s="87"/>
@@ -25870,30 +25889,30 @@
       <c r="BE59" s="87"/>
       <c r="BF59" s="87"/>
       <c r="BG59" s="87"/>
-      <c r="BH59" s="66"/>
-      <c r="BI59" s="67"/>
-      <c r="BJ59" s="67"/>
-      <c r="BK59" s="67"/>
-      <c r="BL59" s="67"/>
-      <c r="BM59" s="67"/>
-      <c r="BN59" s="67"/>
-      <c r="BO59" s="67"/>
-      <c r="BP59" s="66"/>
-      <c r="BQ59" s="68"/>
-      <c r="BR59" s="68"/>
-      <c r="BS59" s="68"/>
-      <c r="BT59" s="68"/>
-      <c r="BU59" s="68"/>
-      <c r="BV59" s="68"/>
-      <c r="BW59" s="68"/>
-      <c r="BX59" s="66"/>
-      <c r="BY59" s="68"/>
-      <c r="BZ59" s="68"/>
-      <c r="CA59" s="68"/>
-      <c r="CB59" s="68"/>
-      <c r="CC59" s="68"/>
-      <c r="CD59" s="68"/>
-      <c r="CE59" s="68"/>
+      <c r="BH59" s="36"/>
+      <c r="BI59" s="37"/>
+      <c r="BJ59" s="37"/>
+      <c r="BK59" s="37"/>
+      <c r="BL59" s="37"/>
+      <c r="BM59" s="37"/>
+      <c r="BN59" s="37"/>
+      <c r="BO59" s="37"/>
+      <c r="BP59" s="36"/>
+      <c r="BQ59" s="45"/>
+      <c r="BR59" s="45"/>
+      <c r="BS59" s="45"/>
+      <c r="BT59" s="45"/>
+      <c r="BU59" s="45"/>
+      <c r="BV59" s="45"/>
+      <c r="BW59" s="45"/>
+      <c r="BX59" s="36"/>
+      <c r="BY59" s="45"/>
+      <c r="BZ59" s="45"/>
+      <c r="CA59" s="45"/>
+      <c r="CB59" s="45"/>
+      <c r="CC59" s="45"/>
+      <c r="CD59" s="45"/>
+      <c r="CE59" s="45"/>
       <c r="CF59" s="86"/>
       <c r="CG59" s="87"/>
       <c r="CH59" s="87"/>
@@ -25926,75 +25945,77 @@
       <c r="DI59" s="87"/>
       <c r="DJ59" s="87"/>
       <c r="DK59" s="87"/>
-      <c r="DL59" s="66"/>
-      <c r="DM59" s="68"/>
-      <c r="DN59" s="68"/>
-      <c r="DO59" s="68"/>
-      <c r="DP59" s="68"/>
-      <c r="DQ59" s="68"/>
-      <c r="DR59" s="68"/>
-      <c r="DS59" s="68"/>
-      <c r="DT59" s="66"/>
-      <c r="DU59" s="68"/>
-      <c r="DV59" s="68"/>
-      <c r="DW59" s="68"/>
-      <c r="DX59" s="68"/>
-      <c r="DY59" s="68"/>
-      <c r="DZ59" s="68"/>
-      <c r="EA59" s="68"/>
-      <c r="EB59" s="66"/>
-      <c r="EC59" s="67"/>
-      <c r="ED59" s="68"/>
-      <c r="EE59" s="68"/>
-      <c r="EF59" s="68"/>
-      <c r="EG59" s="68"/>
-      <c r="EH59" s="68"/>
-      <c r="EI59" s="68"/>
-      <c r="EJ59" s="66"/>
-      <c r="EK59" s="67"/>
-      <c r="EL59" s="68"/>
-      <c r="EM59" s="68"/>
-      <c r="EN59" s="68"/>
-      <c r="EO59" s="68"/>
-      <c r="EP59" s="68"/>
-      <c r="EQ59" s="74"/>
+      <c r="DL59" s="36"/>
+      <c r="DM59" s="45"/>
+      <c r="DN59" s="45"/>
+      <c r="DO59" s="45"/>
+      <c r="DP59" s="45"/>
+      <c r="DQ59" s="45"/>
+      <c r="DR59" s="45"/>
+      <c r="DS59" s="45"/>
+      <c r="DT59" s="36"/>
+      <c r="DU59" s="45"/>
+      <c r="DV59" s="45"/>
+      <c r="DW59" s="45"/>
+      <c r="DX59" s="45"/>
+      <c r="DY59" s="45"/>
+      <c r="DZ59" s="45"/>
+      <c r="EA59" s="45"/>
+      <c r="EB59" s="36"/>
+      <c r="EC59" s="37"/>
+      <c r="ED59" s="45"/>
+      <c r="EE59" s="45"/>
+      <c r="EF59" s="45"/>
+      <c r="EG59" s="45"/>
+      <c r="EH59" s="45"/>
+      <c r="EI59" s="45"/>
+      <c r="EJ59" s="36"/>
+      <c r="EK59" s="37"/>
+      <c r="EL59" s="45"/>
+      <c r="EM59" s="45"/>
+      <c r="EN59" s="45"/>
+      <c r="EO59" s="45"/>
+      <c r="EP59" s="45"/>
+      <c r="EQ59" s="73"/>
     </row>
     <row r="60" spans="1:147" x14ac:dyDescent="0.25">
-      <c r="A60" s="64"/>
-      <c r="B60" s="65"/>
-      <c r="C60" s="48"/>
-      <c r="D60" s="66"/>
-      <c r="E60" s="67"/>
-      <c r="F60" s="67"/>
-      <c r="G60" s="67"/>
-      <c r="H60" s="67"/>
-      <c r="I60" s="67"/>
-      <c r="J60" s="67"/>
-      <c r="K60" s="67"/>
-      <c r="L60" s="66"/>
-      <c r="M60" s="68"/>
-      <c r="N60" s="68"/>
-      <c r="O60" s="68"/>
-      <c r="P60" s="68"/>
-      <c r="Q60" s="68"/>
-      <c r="R60" s="68"/>
-      <c r="S60" s="68"/>
-      <c r="T60" s="66"/>
-      <c r="U60" s="68"/>
-      <c r="V60" s="68"/>
-      <c r="W60" s="68"/>
-      <c r="X60" s="68"/>
-      <c r="Y60" s="68"/>
-      <c r="Z60" s="68"/>
-      <c r="AA60" s="68"/>
-      <c r="AB60" s="66"/>
-      <c r="AC60" s="68"/>
-      <c r="AD60" s="68"/>
-      <c r="AE60" s="68"/>
-      <c r="AF60" s="68"/>
-      <c r="AG60" s="68"/>
-      <c r="AH60" s="68"/>
-      <c r="AI60" s="68"/>
+      <c r="A60" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B60" s="61"/>
+      <c r="C60" s="13"/>
+      <c r="D60" s="5"/>
+      <c r="E60" s="4"/>
+      <c r="F60" s="4"/>
+      <c r="G60" s="4"/>
+      <c r="H60" s="4"/>
+      <c r="I60" s="4"/>
+      <c r="J60" s="4"/>
+      <c r="K60" s="4"/>
+      <c r="L60" s="5"/>
+      <c r="M60" s="42"/>
+      <c r="N60" s="42"/>
+      <c r="O60" s="42"/>
+      <c r="P60" s="42"/>
+      <c r="Q60" s="42"/>
+      <c r="R60" s="42"/>
+      <c r="S60" s="42"/>
+      <c r="T60" s="5"/>
+      <c r="U60" s="42"/>
+      <c r="V60" s="42"/>
+      <c r="W60" s="42"/>
+      <c r="X60" s="42"/>
+      <c r="Y60" s="42"/>
+      <c r="Z60" s="42"/>
+      <c r="AA60" s="42"/>
+      <c r="AB60" s="5"/>
+      <c r="AC60" s="42"/>
+      <c r="AD60" s="42"/>
+      <c r="AE60" s="42"/>
+      <c r="AF60" s="42"/>
+      <c r="AG60" s="42"/>
+      <c r="AH60" s="42"/>
+      <c r="AI60" s="42"/>
       <c r="AJ60" s="86"/>
       <c r="AK60" s="87"/>
       <c r="AL60" s="87"/>
@@ -26019,30 +26040,30 @@
       <c r="BE60" s="87"/>
       <c r="BF60" s="87"/>
       <c r="BG60" s="87"/>
-      <c r="BH60" s="66"/>
-      <c r="BI60" s="67"/>
-      <c r="BJ60" s="67"/>
-      <c r="BK60" s="67"/>
-      <c r="BL60" s="67"/>
-      <c r="BM60" s="67"/>
-      <c r="BN60" s="67"/>
-      <c r="BO60" s="67"/>
-      <c r="BP60" s="66"/>
-      <c r="BQ60" s="68"/>
-      <c r="BR60" s="68"/>
-      <c r="BS60" s="68"/>
-      <c r="BT60" s="68"/>
-      <c r="BU60" s="68"/>
-      <c r="BV60" s="68"/>
-      <c r="BW60" s="68"/>
-      <c r="BX60" s="66"/>
-      <c r="BY60" s="68"/>
-      <c r="BZ60" s="68"/>
-      <c r="CA60" s="68"/>
-      <c r="CB60" s="68"/>
-      <c r="CC60" s="68"/>
-      <c r="CD60" s="68"/>
-      <c r="CE60" s="68"/>
+      <c r="BH60" s="5"/>
+      <c r="BI60" s="4"/>
+      <c r="BJ60" s="4"/>
+      <c r="BK60" s="4"/>
+      <c r="BL60" s="4"/>
+      <c r="BM60" s="4"/>
+      <c r="BN60" s="4"/>
+      <c r="BO60" s="4"/>
+      <c r="BP60" s="5"/>
+      <c r="BQ60" s="42"/>
+      <c r="BR60" s="42"/>
+      <c r="BS60" s="42"/>
+      <c r="BT60" s="42"/>
+      <c r="BU60" s="42"/>
+      <c r="BV60" s="42"/>
+      <c r="BW60" s="42"/>
+      <c r="BX60" s="5"/>
+      <c r="BY60" s="42"/>
+      <c r="BZ60" s="42"/>
+      <c r="CA60" s="42"/>
+      <c r="CB60" s="42"/>
+      <c r="CC60" s="42"/>
+      <c r="CD60" s="42"/>
+      <c r="CE60" s="42"/>
       <c r="CF60" s="86"/>
       <c r="CG60" s="87"/>
       <c r="CH60" s="87"/>
@@ -26075,78 +26096,80 @@
       <c r="DI60" s="87"/>
       <c r="DJ60" s="87"/>
       <c r="DK60" s="87"/>
-      <c r="DL60" s="66"/>
-      <c r="DM60" s="68"/>
-      <c r="DN60" s="68"/>
-      <c r="DO60" s="68"/>
-      <c r="DP60" s="68"/>
-      <c r="DQ60" s="68"/>
-      <c r="DR60" s="68"/>
-      <c r="DS60" s="68"/>
-      <c r="DT60" s="66"/>
-      <c r="DU60" s="68"/>
-      <c r="DV60" s="68"/>
-      <c r="DW60" s="68"/>
-      <c r="DX60" s="68"/>
-      <c r="DY60" s="68"/>
-      <c r="DZ60" s="68"/>
-      <c r="EA60" s="68"/>
-      <c r="EB60" s="66"/>
-      <c r="EC60" s="67"/>
-      <c r="ED60" s="68"/>
-      <c r="EE60" s="68"/>
-      <c r="EF60" s="68"/>
-      <c r="EG60" s="68"/>
-      <c r="EH60" s="68"/>
-      <c r="EI60" s="68"/>
-      <c r="EJ60" s="66"/>
-      <c r="EK60" s="67"/>
-      <c r="EL60" s="68"/>
-      <c r="EM60" s="68"/>
-      <c r="EN60" s="68"/>
-      <c r="EO60" s="68"/>
-      <c r="EP60" s="68"/>
-      <c r="EQ60" s="74"/>
+      <c r="DL60" s="5"/>
+      <c r="DM60" s="42"/>
+      <c r="DN60" s="42"/>
+      <c r="DO60" s="42"/>
+      <c r="DP60" s="42"/>
+      <c r="DQ60" s="42"/>
+      <c r="DR60" s="42"/>
+      <c r="DS60" s="42"/>
+      <c r="DT60" s="5"/>
+      <c r="DU60" s="42"/>
+      <c r="DV60" s="42"/>
+      <c r="DW60" s="42"/>
+      <c r="DX60" s="42"/>
+      <c r="DY60" s="42"/>
+      <c r="DZ60" s="42"/>
+      <c r="EA60" s="42"/>
+      <c r="EB60" s="5"/>
+      <c r="EC60" s="4"/>
+      <c r="ED60" s="42"/>
+      <c r="EE60" s="42"/>
+      <c r="EF60" s="42"/>
+      <c r="EG60" s="42"/>
+      <c r="EH60" s="42"/>
+      <c r="EI60" s="42"/>
+      <c r="EJ60" s="5"/>
+      <c r="EK60" s="4"/>
+      <c r="EL60" s="42"/>
+      <c r="EM60" s="42"/>
+      <c r="EN60" s="42"/>
+      <c r="EO60" s="42"/>
+      <c r="EP60" s="42"/>
+      <c r="EQ60" s="70"/>
     </row>
-    <row r="61" spans="1:147" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="17"/>
-      <c r="B61" s="60"/>
-      <c r="C61" s="50" t="str">
-        <f>IF($B61&gt;"",SUM(COUNTIF($D61:$EQ61,"R")),"")</f>
-        <v/>
-      </c>
-      <c r="D61" s="36"/>
-      <c r="E61" s="37"/>
-      <c r="F61" s="37"/>
-      <c r="G61" s="37"/>
-      <c r="H61" s="37"/>
-      <c r="I61" s="37"/>
-      <c r="J61" s="37"/>
-      <c r="K61" s="37"/>
-      <c r="L61" s="36"/>
-      <c r="M61" s="45"/>
-      <c r="N61" s="45"/>
-      <c r="O61" s="45"/>
-      <c r="P61" s="45"/>
-      <c r="Q61" s="45"/>
-      <c r="R61" s="45"/>
-      <c r="S61" s="45"/>
-      <c r="T61" s="36"/>
-      <c r="U61" s="45"/>
-      <c r="V61" s="45"/>
-      <c r="W61" s="45"/>
-      <c r="X61" s="45"/>
-      <c r="Y61" s="45"/>
-      <c r="Z61" s="45"/>
-      <c r="AA61" s="45"/>
-      <c r="AB61" s="36"/>
-      <c r="AC61" s="45"/>
-      <c r="AD61" s="45"/>
-      <c r="AE61" s="45"/>
-      <c r="AF61" s="45"/>
-      <c r="AG61" s="45"/>
-      <c r="AH61" s="45"/>
-      <c r="AI61" s="45"/>
+    <row r="61" spans="1:147" x14ac:dyDescent="0.25">
+      <c r="A61" s="16"/>
+      <c r="B61" s="55" t="s">
+        <v>45</v>
+      </c>
+      <c r="C61" s="9">
+        <f t="shared" ref="C61:C70" si="5">IF($B61&gt;"",SUM(COUNTIF($D61:$EQ61,"R")),"")</f>
+        <v>0</v>
+      </c>
+      <c r="D61" s="32"/>
+      <c r="E61" s="33"/>
+      <c r="F61" s="33"/>
+      <c r="G61" s="33"/>
+      <c r="H61" s="33"/>
+      <c r="I61" s="33"/>
+      <c r="J61" s="33"/>
+      <c r="K61" s="33"/>
+      <c r="L61" s="32"/>
+      <c r="M61" s="43"/>
+      <c r="N61" s="43"/>
+      <c r="O61" s="43"/>
+      <c r="P61" s="43"/>
+      <c r="Q61" s="43"/>
+      <c r="R61" s="43"/>
+      <c r="S61" s="43"/>
+      <c r="T61" s="32"/>
+      <c r="U61" s="43"/>
+      <c r="V61" s="43"/>
+      <c r="W61" s="43"/>
+      <c r="X61" s="43"/>
+      <c r="Y61" s="43"/>
+      <c r="Z61" s="43"/>
+      <c r="AA61" s="43"/>
+      <c r="AB61" s="32"/>
+      <c r="AC61" s="43"/>
+      <c r="AD61" s="43"/>
+      <c r="AE61" s="43"/>
+      <c r="AF61" s="43"/>
+      <c r="AG61" s="43"/>
+      <c r="AH61" s="43"/>
+      <c r="AI61" s="43"/>
       <c r="AJ61" s="86"/>
       <c r="AK61" s="87"/>
       <c r="AL61" s="87"/>
@@ -26171,30 +26194,30 @@
       <c r="BE61" s="87"/>
       <c r="BF61" s="87"/>
       <c r="BG61" s="87"/>
-      <c r="BH61" s="36"/>
-      <c r="BI61" s="37"/>
-      <c r="BJ61" s="37"/>
-      <c r="BK61" s="37"/>
-      <c r="BL61" s="37"/>
-      <c r="BM61" s="37"/>
-      <c r="BN61" s="37"/>
-      <c r="BO61" s="37"/>
-      <c r="BP61" s="36"/>
-      <c r="BQ61" s="45"/>
-      <c r="BR61" s="45"/>
-      <c r="BS61" s="45"/>
-      <c r="BT61" s="45"/>
-      <c r="BU61" s="45"/>
-      <c r="BV61" s="45"/>
-      <c r="BW61" s="45"/>
-      <c r="BX61" s="36"/>
-      <c r="BY61" s="45"/>
-      <c r="BZ61" s="45"/>
-      <c r="CA61" s="45"/>
-      <c r="CB61" s="45"/>
-      <c r="CC61" s="45"/>
-      <c r="CD61" s="45"/>
-      <c r="CE61" s="45"/>
+      <c r="BH61" s="32"/>
+      <c r="BI61" s="33"/>
+      <c r="BJ61" s="33"/>
+      <c r="BK61" s="33"/>
+      <c r="BL61" s="33"/>
+      <c r="BM61" s="33"/>
+      <c r="BN61" s="33"/>
+      <c r="BO61" s="33"/>
+      <c r="BP61" s="32"/>
+      <c r="BQ61" s="43"/>
+      <c r="BR61" s="43"/>
+      <c r="BS61" s="43"/>
+      <c r="BT61" s="43"/>
+      <c r="BU61" s="43"/>
+      <c r="BV61" s="43"/>
+      <c r="BW61" s="43"/>
+      <c r="BX61" s="32"/>
+      <c r="BY61" s="43"/>
+      <c r="BZ61" s="43"/>
+      <c r="CA61" s="43"/>
+      <c r="CB61" s="43"/>
+      <c r="CC61" s="43"/>
+      <c r="CD61" s="43"/>
+      <c r="CE61" s="43"/>
       <c r="CF61" s="86"/>
       <c r="CG61" s="87"/>
       <c r="CH61" s="87"/>
@@ -26227,77 +26250,80 @@
       <c r="DI61" s="87"/>
       <c r="DJ61" s="87"/>
       <c r="DK61" s="87"/>
-      <c r="DL61" s="36"/>
-      <c r="DM61" s="45"/>
-      <c r="DN61" s="45"/>
-      <c r="DO61" s="45"/>
-      <c r="DP61" s="45"/>
-      <c r="DQ61" s="45"/>
-      <c r="DR61" s="45"/>
-      <c r="DS61" s="45"/>
-      <c r="DT61" s="36"/>
-      <c r="DU61" s="45"/>
-      <c r="DV61" s="45"/>
-      <c r="DW61" s="45"/>
-      <c r="DX61" s="45"/>
-      <c r="DY61" s="45"/>
-      <c r="DZ61" s="45"/>
-      <c r="EA61" s="45"/>
-      <c r="EB61" s="36"/>
-      <c r="EC61" s="37"/>
-      <c r="ED61" s="45"/>
-      <c r="EE61" s="45"/>
-      <c r="EF61" s="45"/>
-      <c r="EG61" s="45"/>
-      <c r="EH61" s="45"/>
-      <c r="EI61" s="45"/>
-      <c r="EJ61" s="36"/>
-      <c r="EK61" s="37"/>
-      <c r="EL61" s="45"/>
-      <c r="EM61" s="45"/>
-      <c r="EN61" s="45"/>
-      <c r="EO61" s="45"/>
-      <c r="EP61" s="45"/>
-      <c r="EQ61" s="73"/>
+      <c r="DL61" s="32"/>
+      <c r="DM61" s="43"/>
+      <c r="DN61" s="43"/>
+      <c r="DO61" s="43"/>
+      <c r="DP61" s="43"/>
+      <c r="DQ61" s="43"/>
+      <c r="DR61" s="43"/>
+      <c r="DS61" s="43"/>
+      <c r="DT61" s="32"/>
+      <c r="DU61" s="43"/>
+      <c r="DV61" s="43"/>
+      <c r="DW61" s="43"/>
+      <c r="DX61" s="43"/>
+      <c r="DY61" s="43"/>
+      <c r="DZ61" s="43"/>
+      <c r="EA61" s="43"/>
+      <c r="EB61" s="32"/>
+      <c r="EC61" s="33"/>
+      <c r="ED61" s="43"/>
+      <c r="EE61" s="43"/>
+      <c r="EF61" s="43"/>
+      <c r="EG61" s="43"/>
+      <c r="EH61" s="43"/>
+      <c r="EI61" s="43"/>
+      <c r="EJ61" s="32"/>
+      <c r="EK61" s="33"/>
+      <c r="EL61" s="43"/>
+      <c r="EM61" s="43"/>
+      <c r="EN61" s="43"/>
+      <c r="EO61" s="43"/>
+      <c r="EP61" s="43"/>
+      <c r="EQ61" s="71"/>
     </row>
     <row r="62" spans="1:147" x14ac:dyDescent="0.25">
-      <c r="A62" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="B62" s="61"/>
-      <c r="C62" s="13"/>
-      <c r="D62" s="5"/>
-      <c r="E62" s="4"/>
-      <c r="F62" s="4"/>
-      <c r="G62" s="4"/>
-      <c r="H62" s="4"/>
-      <c r="I62" s="4"/>
-      <c r="J62" s="4"/>
-      <c r="K62" s="4"/>
-      <c r="L62" s="5"/>
-      <c r="M62" s="42"/>
-      <c r="N62" s="42"/>
-      <c r="O62" s="42"/>
-      <c r="P62" s="42"/>
-      <c r="Q62" s="42"/>
-      <c r="R62" s="42"/>
-      <c r="S62" s="42"/>
-      <c r="T62" s="5"/>
-      <c r="U62" s="42"/>
-      <c r="V62" s="42"/>
-      <c r="W62" s="42"/>
-      <c r="X62" s="42"/>
-      <c r="Y62" s="42"/>
-      <c r="Z62" s="42"/>
-      <c r="AA62" s="42"/>
-      <c r="AB62" s="5"/>
-      <c r="AC62" s="42"/>
-      <c r="AD62" s="42"/>
-      <c r="AE62" s="42"/>
-      <c r="AF62" s="42"/>
-      <c r="AG62" s="42"/>
-      <c r="AH62" s="42"/>
-      <c r="AI62" s="42"/>
+      <c r="A62" s="16"/>
+      <c r="B62" s="55" t="s">
+        <v>46</v>
+      </c>
+      <c r="C62" s="9">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="D62" s="34"/>
+      <c r="E62" s="35"/>
+      <c r="F62" s="35"/>
+      <c r="G62" s="35"/>
+      <c r="H62" s="35"/>
+      <c r="I62" s="35"/>
+      <c r="J62" s="35"/>
+      <c r="K62" s="35"/>
+      <c r="L62" s="34"/>
+      <c r="M62" s="35"/>
+      <c r="N62" s="35"/>
+      <c r="O62" s="35"/>
+      <c r="P62" s="35"/>
+      <c r="Q62" s="35"/>
+      <c r="R62" s="35"/>
+      <c r="S62" s="35"/>
+      <c r="T62" s="34"/>
+      <c r="U62" s="35"/>
+      <c r="V62" s="35"/>
+      <c r="W62" s="35"/>
+      <c r="X62" s="35"/>
+      <c r="Y62" s="35"/>
+      <c r="Z62" s="35"/>
+      <c r="AA62" s="35"/>
+      <c r="AB62" s="34"/>
+      <c r="AC62" s="35"/>
+      <c r="AD62" s="35"/>
+      <c r="AE62" s="35"/>
+      <c r="AF62" s="35"/>
+      <c r="AG62" s="35"/>
+      <c r="AH62" s="35"/>
+      <c r="AI62" s="35"/>
       <c r="AJ62" s="86"/>
       <c r="AK62" s="87"/>
       <c r="AL62" s="87"/>
@@ -26322,30 +26348,30 @@
       <c r="BE62" s="87"/>
       <c r="BF62" s="87"/>
       <c r="BG62" s="87"/>
-      <c r="BH62" s="5"/>
-      <c r="BI62" s="4"/>
-      <c r="BJ62" s="4"/>
-      <c r="BK62" s="4"/>
-      <c r="BL62" s="4"/>
-      <c r="BM62" s="4"/>
-      <c r="BN62" s="4"/>
-      <c r="BO62" s="4"/>
-      <c r="BP62" s="5"/>
-      <c r="BQ62" s="42"/>
-      <c r="BR62" s="42"/>
-      <c r="BS62" s="42"/>
-      <c r="BT62" s="42"/>
-      <c r="BU62" s="42"/>
-      <c r="BV62" s="42"/>
-      <c r="BW62" s="42"/>
-      <c r="BX62" s="5"/>
-      <c r="BY62" s="42"/>
-      <c r="BZ62" s="42"/>
-      <c r="CA62" s="42"/>
-      <c r="CB62" s="42"/>
-      <c r="CC62" s="42"/>
-      <c r="CD62" s="42"/>
-      <c r="CE62" s="42"/>
+      <c r="BH62" s="34"/>
+      <c r="BI62" s="35"/>
+      <c r="BJ62" s="35"/>
+      <c r="BK62" s="35"/>
+      <c r="BL62" s="35"/>
+      <c r="BM62" s="35"/>
+      <c r="BN62" s="35"/>
+      <c r="BO62" s="35"/>
+      <c r="BP62" s="32"/>
+      <c r="BQ62" s="43"/>
+      <c r="BR62" s="43"/>
+      <c r="BS62" s="43"/>
+      <c r="BT62" s="43"/>
+      <c r="BU62" s="43"/>
+      <c r="BV62" s="43"/>
+      <c r="BW62" s="43"/>
+      <c r="BX62" s="32"/>
+      <c r="BY62" s="43"/>
+      <c r="BZ62" s="43"/>
+      <c r="CA62" s="43"/>
+      <c r="CB62" s="35"/>
+      <c r="CC62" s="35"/>
+      <c r="CD62" s="35"/>
+      <c r="CE62" s="35"/>
       <c r="CF62" s="86"/>
       <c r="CG62" s="87"/>
       <c r="CH62" s="87"/>
@@ -26378,80 +26404,80 @@
       <c r="DI62" s="87"/>
       <c r="DJ62" s="87"/>
       <c r="DK62" s="87"/>
-      <c r="DL62" s="5"/>
-      <c r="DM62" s="42"/>
-      <c r="DN62" s="42"/>
-      <c r="DO62" s="42"/>
-      <c r="DP62" s="42"/>
-      <c r="DQ62" s="42"/>
-      <c r="DR62" s="42"/>
-      <c r="DS62" s="42"/>
-      <c r="DT62" s="5"/>
-      <c r="DU62" s="42"/>
-      <c r="DV62" s="42"/>
-      <c r="DW62" s="42"/>
-      <c r="DX62" s="42"/>
-      <c r="DY62" s="42"/>
-      <c r="DZ62" s="42"/>
-      <c r="EA62" s="42"/>
-      <c r="EB62" s="5"/>
-      <c r="EC62" s="4"/>
-      <c r="ED62" s="42"/>
-      <c r="EE62" s="42"/>
-      <c r="EF62" s="42"/>
-      <c r="EG62" s="42"/>
-      <c r="EH62" s="42"/>
-      <c r="EI62" s="42"/>
-      <c r="EJ62" s="5"/>
-      <c r="EK62" s="4"/>
-      <c r="EL62" s="42"/>
-      <c r="EM62" s="42"/>
-      <c r="EN62" s="42"/>
-      <c r="EO62" s="42"/>
-      <c r="EP62" s="42"/>
-      <c r="EQ62" s="70"/>
+      <c r="DL62" s="34"/>
+      <c r="DM62" s="35"/>
+      <c r="DN62" s="35"/>
+      <c r="DO62" s="35"/>
+      <c r="DP62" s="35"/>
+      <c r="DQ62" s="35"/>
+      <c r="DR62" s="35"/>
+      <c r="DS62" s="35"/>
+      <c r="DT62" s="34"/>
+      <c r="DU62" s="35"/>
+      <c r="DV62" s="35"/>
+      <c r="DW62" s="35"/>
+      <c r="DX62" s="35"/>
+      <c r="DY62" s="35"/>
+      <c r="DZ62" s="35"/>
+      <c r="EA62" s="35"/>
+      <c r="EB62" s="34"/>
+      <c r="EC62" s="35"/>
+      <c r="ED62" s="35"/>
+      <c r="EE62" s="35"/>
+      <c r="EF62" s="35"/>
+      <c r="EG62" s="35"/>
+      <c r="EH62" s="35"/>
+      <c r="EI62" s="35"/>
+      <c r="EJ62" s="34"/>
+      <c r="EK62" s="35"/>
+      <c r="EL62" s="35"/>
+      <c r="EM62" s="35"/>
+      <c r="EN62" s="35"/>
+      <c r="EO62" s="35"/>
+      <c r="EP62" s="35"/>
+      <c r="EQ62" s="72"/>
     </row>
     <row r="63" spans="1:147" x14ac:dyDescent="0.25">
       <c r="A63" s="16"/>
       <c r="B63" s="55" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C63" s="9">
-        <f t="shared" ref="C63:C72" si="5">IF($B63&gt;"",SUM(COUNTIF($D63:$EQ63,"R")),"")</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="D63" s="32"/>
-      <c r="E63" s="33"/>
-      <c r="F63" s="33"/>
-      <c r="G63" s="33"/>
-      <c r="H63" s="33"/>
-      <c r="I63" s="33"/>
-      <c r="J63" s="33"/>
-      <c r="K63" s="33"/>
-      <c r="L63" s="32"/>
-      <c r="M63" s="43"/>
-      <c r="N63" s="43"/>
-      <c r="O63" s="43"/>
-      <c r="P63" s="43"/>
-      <c r="Q63" s="43"/>
-      <c r="R63" s="43"/>
-      <c r="S63" s="43"/>
-      <c r="T63" s="32"/>
-      <c r="U63" s="43"/>
-      <c r="V63" s="43"/>
-      <c r="W63" s="43"/>
-      <c r="X63" s="43"/>
-      <c r="Y63" s="43"/>
-      <c r="Z63" s="43"/>
-      <c r="AA63" s="43"/>
-      <c r="AB63" s="32"/>
-      <c r="AC63" s="43"/>
-      <c r="AD63" s="43"/>
-      <c r="AE63" s="43"/>
-      <c r="AF63" s="43"/>
-      <c r="AG63" s="43"/>
-      <c r="AH63" s="43"/>
-      <c r="AI63" s="43"/>
+      <c r="D63" s="34"/>
+      <c r="E63" s="35"/>
+      <c r="F63" s="35"/>
+      <c r="G63" s="35"/>
+      <c r="H63" s="35"/>
+      <c r="I63" s="35"/>
+      <c r="J63" s="35"/>
+      <c r="K63" s="35"/>
+      <c r="L63" s="34"/>
+      <c r="M63" s="44"/>
+      <c r="N63" s="44"/>
+      <c r="O63" s="44"/>
+      <c r="P63" s="44"/>
+      <c r="Q63" s="44"/>
+      <c r="R63" s="44"/>
+      <c r="S63" s="44"/>
+      <c r="T63" s="34"/>
+      <c r="U63" s="44"/>
+      <c r="V63" s="44"/>
+      <c r="W63" s="44"/>
+      <c r="X63" s="44"/>
+      <c r="Y63" s="44"/>
+      <c r="Z63" s="44"/>
+      <c r="AA63" s="44"/>
+      <c r="AB63" s="34"/>
+      <c r="AC63" s="44"/>
+      <c r="AD63" s="44"/>
+      <c r="AE63" s="44"/>
+      <c r="AF63" s="44"/>
+      <c r="AG63" s="44"/>
+      <c r="AH63" s="44"/>
+      <c r="AI63" s="44"/>
       <c r="AJ63" s="86"/>
       <c r="AK63" s="87"/>
       <c r="AL63" s="87"/>
@@ -26476,14 +26502,14 @@
       <c r="BE63" s="87"/>
       <c r="BF63" s="87"/>
       <c r="BG63" s="87"/>
-      <c r="BH63" s="32"/>
-      <c r="BI63" s="33"/>
-      <c r="BJ63" s="33"/>
-      <c r="BK63" s="33"/>
-      <c r="BL63" s="33"/>
-      <c r="BM63" s="33"/>
-      <c r="BN63" s="33"/>
-      <c r="BO63" s="33"/>
+      <c r="BH63" s="34"/>
+      <c r="BI63" s="35"/>
+      <c r="BJ63" s="35"/>
+      <c r="BK63" s="35"/>
+      <c r="BL63" s="35"/>
+      <c r="BM63" s="35"/>
+      <c r="BN63" s="35"/>
+      <c r="BO63" s="35"/>
       <c r="BP63" s="32"/>
       <c r="BQ63" s="43"/>
       <c r="BR63" s="43"/>
@@ -26496,10 +26522,10 @@
       <c r="BY63" s="43"/>
       <c r="BZ63" s="43"/>
       <c r="CA63" s="43"/>
-      <c r="CB63" s="43"/>
-      <c r="CC63" s="43"/>
-      <c r="CD63" s="43"/>
-      <c r="CE63" s="43"/>
+      <c r="CB63" s="44"/>
+      <c r="CC63" s="44"/>
+      <c r="CD63" s="44"/>
+      <c r="CE63" s="44"/>
       <c r="CF63" s="86"/>
       <c r="CG63" s="87"/>
       <c r="CH63" s="87"/>
@@ -26532,43 +26558,43 @@
       <c r="DI63" s="87"/>
       <c r="DJ63" s="87"/>
       <c r="DK63" s="87"/>
-      <c r="DL63" s="32"/>
-      <c r="DM63" s="43"/>
-      <c r="DN63" s="43"/>
-      <c r="DO63" s="43"/>
-      <c r="DP63" s="43"/>
-      <c r="DQ63" s="43"/>
-      <c r="DR63" s="43"/>
-      <c r="DS63" s="43"/>
-      <c r="DT63" s="32"/>
-      <c r="DU63" s="43"/>
-      <c r="DV63" s="43"/>
-      <c r="DW63" s="43"/>
-      <c r="DX63" s="43"/>
-      <c r="DY63" s="43"/>
-      <c r="DZ63" s="43"/>
-      <c r="EA63" s="43"/>
-      <c r="EB63" s="32"/>
-      <c r="EC63" s="33"/>
-      <c r="ED63" s="43"/>
-      <c r="EE63" s="43"/>
-      <c r="EF63" s="43"/>
-      <c r="EG63" s="43"/>
-      <c r="EH63" s="43"/>
-      <c r="EI63" s="43"/>
-      <c r="EJ63" s="32"/>
-      <c r="EK63" s="33"/>
-      <c r="EL63" s="43"/>
-      <c r="EM63" s="43"/>
-      <c r="EN63" s="43"/>
-      <c r="EO63" s="43"/>
-      <c r="EP63" s="43"/>
-      <c r="EQ63" s="71"/>
+      <c r="DL63" s="34"/>
+      <c r="DM63" s="44"/>
+      <c r="DN63" s="44"/>
+      <c r="DO63" s="44"/>
+      <c r="DP63" s="44"/>
+      <c r="DQ63" s="44"/>
+      <c r="DR63" s="44"/>
+      <c r="DS63" s="44"/>
+      <c r="DT63" s="34"/>
+      <c r="DU63" s="44"/>
+      <c r="DV63" s="44"/>
+      <c r="DW63" s="44"/>
+      <c r="DX63" s="44"/>
+      <c r="DY63" s="44"/>
+      <c r="DZ63" s="44"/>
+      <c r="EA63" s="44"/>
+      <c r="EB63" s="34"/>
+      <c r="EC63" s="35"/>
+      <c r="ED63" s="44"/>
+      <c r="EE63" s="44"/>
+      <c r="EF63" s="44"/>
+      <c r="EG63" s="44"/>
+      <c r="EH63" s="44"/>
+      <c r="EI63" s="44"/>
+      <c r="EJ63" s="34"/>
+      <c r="EK63" s="35"/>
+      <c r="EL63" s="35"/>
+      <c r="EM63" s="35"/>
+      <c r="EN63" s="35"/>
+      <c r="EO63" s="35"/>
+      <c r="EP63" s="35"/>
+      <c r="EQ63" s="72"/>
     </row>
-    <row r="64" spans="1:147" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:147" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" s="16"/>
       <c r="B64" s="55" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C64" s="9">
         <f t="shared" si="5"/>
@@ -26583,29 +26609,29 @@
       <c r="J64" s="35"/>
       <c r="K64" s="35"/>
       <c r="L64" s="34"/>
-      <c r="M64" s="35"/>
-      <c r="N64" s="35"/>
-      <c r="O64" s="35"/>
-      <c r="P64" s="35"/>
-      <c r="Q64" s="35"/>
-      <c r="R64" s="35"/>
-      <c r="S64" s="35"/>
+      <c r="M64" s="44"/>
+      <c r="N64" s="44"/>
+      <c r="O64" s="44"/>
+      <c r="P64" s="44"/>
+      <c r="Q64" s="44"/>
+      <c r="R64" s="44"/>
+      <c r="S64" s="44"/>
       <c r="T64" s="34"/>
-      <c r="U64" s="35"/>
-      <c r="V64" s="35"/>
-      <c r="W64" s="35"/>
-      <c r="X64" s="35"/>
-      <c r="Y64" s="35"/>
-      <c r="Z64" s="35"/>
-      <c r="AA64" s="35"/>
+      <c r="U64" s="44"/>
+      <c r="V64" s="44"/>
+      <c r="W64" s="44"/>
+      <c r="X64" s="44"/>
+      <c r="Y64" s="44"/>
+      <c r="Z64" s="44"/>
+      <c r="AA64" s="44"/>
       <c r="AB64" s="34"/>
-      <c r="AC64" s="35"/>
-      <c r="AD64" s="35"/>
-      <c r="AE64" s="35"/>
-      <c r="AF64" s="35"/>
-      <c r="AG64" s="35"/>
-      <c r="AH64" s="35"/>
-      <c r="AI64" s="35"/>
+      <c r="AC64" s="44"/>
+      <c r="AD64" s="44"/>
+      <c r="AE64" s="44"/>
+      <c r="AF64" s="44"/>
+      <c r="AG64" s="44"/>
+      <c r="AH64" s="44"/>
+      <c r="AI64" s="44"/>
       <c r="AJ64" s="86"/>
       <c r="AK64" s="87"/>
       <c r="AL64" s="87"/>
@@ -26638,22 +26664,22 @@
       <c r="BM64" s="35"/>
       <c r="BN64" s="35"/>
       <c r="BO64" s="35"/>
-      <c r="BP64" s="32"/>
-      <c r="BQ64" s="43"/>
-      <c r="BR64" s="43"/>
-      <c r="BS64" s="43"/>
-      <c r="BT64" s="43"/>
-      <c r="BU64" s="43"/>
-      <c r="BV64" s="43"/>
-      <c r="BW64" s="43"/>
+      <c r="BP64" s="34"/>
+      <c r="BQ64" s="44"/>
+      <c r="BR64" s="44"/>
+      <c r="BS64" s="44"/>
+      <c r="BT64" s="44"/>
+      <c r="BU64" s="44"/>
+      <c r="BV64" s="44"/>
+      <c r="BW64" s="35"/>
       <c r="BX64" s="32"/>
       <c r="BY64" s="43"/>
       <c r="BZ64" s="43"/>
       <c r="CA64" s="43"/>
-      <c r="CB64" s="35"/>
-      <c r="CC64" s="35"/>
-      <c r="CD64" s="35"/>
-      <c r="CE64" s="35"/>
+      <c r="CB64" s="44"/>
+      <c r="CC64" s="44"/>
+      <c r="CD64" s="44"/>
+      <c r="CE64" s="44"/>
       <c r="CF64" s="86"/>
       <c r="CG64" s="87"/>
       <c r="CH64" s="87"/>
@@ -26687,46 +26713,44 @@
       <c r="DJ64" s="87"/>
       <c r="DK64" s="87"/>
       <c r="DL64" s="34"/>
-      <c r="DM64" s="35"/>
-      <c r="DN64" s="35"/>
-      <c r="DO64" s="35"/>
-      <c r="DP64" s="35"/>
-      <c r="DQ64" s="35"/>
-      <c r="DR64" s="35"/>
-      <c r="DS64" s="35"/>
+      <c r="DM64" s="44"/>
+      <c r="DN64" s="44"/>
+      <c r="DO64" s="44"/>
+      <c r="DP64" s="44"/>
+      <c r="DQ64" s="44"/>
+      <c r="DR64" s="44"/>
+      <c r="DS64" s="44"/>
       <c r="DT64" s="34"/>
-      <c r="DU64" s="35"/>
-      <c r="DV64" s="35"/>
-      <c r="DW64" s="35"/>
-      <c r="DX64" s="35"/>
-      <c r="DY64" s="35"/>
-      <c r="DZ64" s="35"/>
-      <c r="EA64" s="35"/>
+      <c r="DU64" s="44"/>
+      <c r="DV64" s="44"/>
+      <c r="DW64" s="44"/>
+      <c r="DX64" s="44"/>
+      <c r="DY64" s="44"/>
+      <c r="DZ64" s="44"/>
+      <c r="EA64" s="44"/>
       <c r="EB64" s="34"/>
       <c r="EC64" s="35"/>
-      <c r="ED64" s="35"/>
-      <c r="EE64" s="35"/>
-      <c r="EF64" s="35"/>
-      <c r="EG64" s="35"/>
-      <c r="EH64" s="35"/>
-      <c r="EI64" s="35"/>
+      <c r="ED64" s="44"/>
+      <c r="EE64" s="44"/>
+      <c r="EF64" s="44"/>
+      <c r="EG64" s="44"/>
+      <c r="EH64" s="44"/>
+      <c r="EI64" s="44"/>
       <c r="EJ64" s="34"/>
       <c r="EK64" s="35"/>
-      <c r="EL64" s="35"/>
-      <c r="EM64" s="35"/>
-      <c r="EN64" s="35"/>
-      <c r="EO64" s="35"/>
-      <c r="EP64" s="35"/>
+      <c r="EL64" s="44"/>
+      <c r="EM64" s="44"/>
+      <c r="EN64" s="44"/>
+      <c r="EO64" s="44"/>
+      <c r="EP64" s="44"/>
       <c r="EQ64" s="72"/>
     </row>
     <row r="65" spans="1:147" x14ac:dyDescent="0.25">
       <c r="A65" s="16"/>
-      <c r="B65" s="55" t="s">
-        <v>47</v>
-      </c>
-      <c r="C65" s="9">
+      <c r="B65" s="55"/>
+      <c r="C65" s="9" t="str">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="D65" s="34"/>
       <c r="E65" s="35"/>
@@ -26792,18 +26816,18 @@
       <c r="BM65" s="35"/>
       <c r="BN65" s="35"/>
       <c r="BO65" s="35"/>
-      <c r="BP65" s="32"/>
-      <c r="BQ65" s="43"/>
-      <c r="BR65" s="43"/>
-      <c r="BS65" s="43"/>
-      <c r="BT65" s="43"/>
-      <c r="BU65" s="43"/>
-      <c r="BV65" s="43"/>
-      <c r="BW65" s="43"/>
-      <c r="BX65" s="32"/>
-      <c r="BY65" s="43"/>
-      <c r="BZ65" s="43"/>
-      <c r="CA65" s="43"/>
+      <c r="BP65" s="34"/>
+      <c r="BQ65" s="44"/>
+      <c r="BR65" s="44"/>
+      <c r="BS65" s="44"/>
+      <c r="BT65" s="44"/>
+      <c r="BU65" s="44"/>
+      <c r="BV65" s="44"/>
+      <c r="BW65" s="44"/>
+      <c r="BX65" s="34"/>
+      <c r="BY65" s="44"/>
+      <c r="BZ65" s="44"/>
+      <c r="CA65" s="44"/>
       <c r="CB65" s="44"/>
       <c r="CC65" s="44"/>
       <c r="CD65" s="44"/>
@@ -26866,21 +26890,19 @@
       <c r="EI65" s="44"/>
       <c r="EJ65" s="34"/>
       <c r="EK65" s="35"/>
-      <c r="EL65" s="35"/>
-      <c r="EM65" s="35"/>
-      <c r="EN65" s="35"/>
-      <c r="EO65" s="35"/>
-      <c r="EP65" s="35"/>
+      <c r="EL65" s="44"/>
+      <c r="EM65" s="44"/>
+      <c r="EN65" s="44"/>
+      <c r="EO65" s="44"/>
+      <c r="EP65" s="44"/>
       <c r="EQ65" s="72"/>
     </row>
-    <row r="66" spans="1:147" ht="30" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:147" x14ac:dyDescent="0.25">
       <c r="A66" s="16"/>
-      <c r="B66" s="55" t="s">
-        <v>48</v>
-      </c>
-      <c r="C66" s="9">
+      <c r="B66" s="55"/>
+      <c r="C66" s="9" t="str">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="D66" s="34"/>
       <c r="E66" s="35"/>
@@ -26953,11 +26975,11 @@
       <c r="BT66" s="44"/>
       <c r="BU66" s="44"/>
       <c r="BV66" s="44"/>
-      <c r="BW66" s="35"/>
-      <c r="BX66" s="32"/>
-      <c r="BY66" s="43"/>
-      <c r="BZ66" s="43"/>
-      <c r="CA66" s="43"/>
+      <c r="BW66" s="44"/>
+      <c r="BX66" s="34"/>
+      <c r="BY66" s="44"/>
+      <c r="BZ66" s="44"/>
+      <c r="CA66" s="44"/>
       <c r="CB66" s="44"/>
       <c r="CC66" s="44"/>
       <c r="CD66" s="44"/>
@@ -27483,45 +27505,45 @@
       <c r="EP69" s="44"/>
       <c r="EQ69" s="72"/>
     </row>
-    <row r="70" spans="1:147" x14ac:dyDescent="0.25">
-      <c r="A70" s="16"/>
-      <c r="B70" s="55"/>
-      <c r="C70" s="9" t="str">
+    <row r="70" spans="1:147" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="17"/>
+      <c r="B70" s="56"/>
+      <c r="C70" s="52" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="D70" s="34"/>
-      <c r="E70" s="35"/>
-      <c r="F70" s="35"/>
-      <c r="G70" s="35"/>
-      <c r="H70" s="35"/>
-      <c r="I70" s="35"/>
-      <c r="J70" s="35"/>
-      <c r="K70" s="35"/>
-      <c r="L70" s="34"/>
-      <c r="M70" s="44"/>
-      <c r="N70" s="44"/>
-      <c r="O70" s="44"/>
-      <c r="P70" s="44"/>
-      <c r="Q70" s="44"/>
-      <c r="R70" s="44"/>
-      <c r="S70" s="44"/>
-      <c r="T70" s="34"/>
-      <c r="U70" s="44"/>
-      <c r="V70" s="44"/>
-      <c r="W70" s="44"/>
-      <c r="X70" s="44"/>
-      <c r="Y70" s="44"/>
-      <c r="Z70" s="44"/>
-      <c r="AA70" s="44"/>
-      <c r="AB70" s="34"/>
-      <c r="AC70" s="44"/>
-      <c r="AD70" s="44"/>
-      <c r="AE70" s="44"/>
-      <c r="AF70" s="44"/>
-      <c r="AG70" s="44"/>
-      <c r="AH70" s="44"/>
-      <c r="AI70" s="44"/>
+      <c r="D70" s="36"/>
+      <c r="E70" s="37"/>
+      <c r="F70" s="37"/>
+      <c r="G70" s="37"/>
+      <c r="H70" s="37"/>
+      <c r="I70" s="37"/>
+      <c r="J70" s="37"/>
+      <c r="K70" s="37"/>
+      <c r="L70" s="36"/>
+      <c r="M70" s="45"/>
+      <c r="N70" s="45"/>
+      <c r="O70" s="45"/>
+      <c r="P70" s="45"/>
+      <c r="Q70" s="45"/>
+      <c r="R70" s="45"/>
+      <c r="S70" s="45"/>
+      <c r="T70" s="36"/>
+      <c r="U70" s="45"/>
+      <c r="V70" s="45"/>
+      <c r="W70" s="45"/>
+      <c r="X70" s="45"/>
+      <c r="Y70" s="45"/>
+      <c r="Z70" s="45"/>
+      <c r="AA70" s="45"/>
+      <c r="AB70" s="36"/>
+      <c r="AC70" s="45"/>
+      <c r="AD70" s="45"/>
+      <c r="AE70" s="45"/>
+      <c r="AF70" s="45"/>
+      <c r="AG70" s="45"/>
+      <c r="AH70" s="45"/>
+      <c r="AI70" s="45"/>
       <c r="AJ70" s="86"/>
       <c r="AK70" s="87"/>
       <c r="AL70" s="87"/>
@@ -27546,30 +27568,30 @@
       <c r="BE70" s="87"/>
       <c r="BF70" s="87"/>
       <c r="BG70" s="87"/>
-      <c r="BH70" s="34"/>
-      <c r="BI70" s="35"/>
-      <c r="BJ70" s="35"/>
-      <c r="BK70" s="35"/>
-      <c r="BL70" s="35"/>
-      <c r="BM70" s="35"/>
-      <c r="BN70" s="35"/>
-      <c r="BO70" s="35"/>
-      <c r="BP70" s="34"/>
-      <c r="BQ70" s="44"/>
-      <c r="BR70" s="44"/>
-      <c r="BS70" s="44"/>
-      <c r="BT70" s="44"/>
-      <c r="BU70" s="44"/>
-      <c r="BV70" s="44"/>
-      <c r="BW70" s="44"/>
-      <c r="BX70" s="34"/>
-      <c r="BY70" s="44"/>
-      <c r="BZ70" s="44"/>
-      <c r="CA70" s="44"/>
-      <c r="CB70" s="44"/>
-      <c r="CC70" s="44"/>
-      <c r="CD70" s="44"/>
-      <c r="CE70" s="44"/>
+      <c r="BH70" s="36"/>
+      <c r="BI70" s="37"/>
+      <c r="BJ70" s="37"/>
+      <c r="BK70" s="37"/>
+      <c r="BL70" s="37"/>
+      <c r="BM70" s="37"/>
+      <c r="BN70" s="37"/>
+      <c r="BO70" s="37"/>
+      <c r="BP70" s="36"/>
+      <c r="BQ70" s="45"/>
+      <c r="BR70" s="45"/>
+      <c r="BS70" s="45"/>
+      <c r="BT70" s="45"/>
+      <c r="BU70" s="45"/>
+      <c r="BV70" s="45"/>
+      <c r="BW70" s="45"/>
+      <c r="BX70" s="36"/>
+      <c r="BY70" s="45"/>
+      <c r="BZ70" s="45"/>
+      <c r="CA70" s="45"/>
+      <c r="CB70" s="45"/>
+      <c r="CC70" s="45"/>
+      <c r="CD70" s="45"/>
+      <c r="CE70" s="45"/>
       <c r="CF70" s="86"/>
       <c r="CG70" s="87"/>
       <c r="CH70" s="87"/>
@@ -27602,78 +27624,77 @@
       <c r="DI70" s="87"/>
       <c r="DJ70" s="87"/>
       <c r="DK70" s="87"/>
-      <c r="DL70" s="34"/>
-      <c r="DM70" s="44"/>
-      <c r="DN70" s="44"/>
-      <c r="DO70" s="44"/>
-      <c r="DP70" s="44"/>
-      <c r="DQ70" s="44"/>
-      <c r="DR70" s="44"/>
-      <c r="DS70" s="44"/>
-      <c r="DT70" s="34"/>
-      <c r="DU70" s="44"/>
-      <c r="DV70" s="44"/>
-      <c r="DW70" s="44"/>
-      <c r="DX70" s="44"/>
-      <c r="DY70" s="44"/>
-      <c r="DZ70" s="44"/>
-      <c r="EA70" s="44"/>
-      <c r="EB70" s="34"/>
-      <c r="EC70" s="35"/>
-      <c r="ED70" s="44"/>
-      <c r="EE70" s="44"/>
-      <c r="EF70" s="44"/>
-      <c r="EG70" s="44"/>
-      <c r="EH70" s="44"/>
-      <c r="EI70" s="44"/>
-      <c r="EJ70" s="34"/>
-      <c r="EK70" s="35"/>
-      <c r="EL70" s="44"/>
-      <c r="EM70" s="44"/>
-      <c r="EN70" s="44"/>
-      <c r="EO70" s="44"/>
-      <c r="EP70" s="44"/>
-      <c r="EQ70" s="72"/>
+      <c r="DL70" s="36"/>
+      <c r="DM70" s="45"/>
+      <c r="DN70" s="45"/>
+      <c r="DO70" s="45"/>
+      <c r="DP70" s="45"/>
+      <c r="DQ70" s="45"/>
+      <c r="DR70" s="45"/>
+      <c r="DS70" s="45"/>
+      <c r="DT70" s="36"/>
+      <c r="DU70" s="45"/>
+      <c r="DV70" s="45"/>
+      <c r="DW70" s="45"/>
+      <c r="DX70" s="45"/>
+      <c r="DY70" s="45"/>
+      <c r="DZ70" s="45"/>
+      <c r="EA70" s="45"/>
+      <c r="EB70" s="36"/>
+      <c r="EC70" s="37"/>
+      <c r="ED70" s="45"/>
+      <c r="EE70" s="45"/>
+      <c r="EF70" s="45"/>
+      <c r="EG70" s="45"/>
+      <c r="EH70" s="45"/>
+      <c r="EI70" s="45"/>
+      <c r="EJ70" s="36"/>
+      <c r="EK70" s="37"/>
+      <c r="EL70" s="45"/>
+      <c r="EM70" s="45"/>
+      <c r="EN70" s="45"/>
+      <c r="EO70" s="45"/>
+      <c r="EP70" s="45"/>
+      <c r="EQ70" s="73"/>
     </row>
     <row r="71" spans="1:147" x14ac:dyDescent="0.25">
-      <c r="A71" s="16"/>
-      <c r="B71" s="55"/>
-      <c r="C71" s="9" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="D71" s="34"/>
-      <c r="E71" s="35"/>
-      <c r="F71" s="35"/>
-      <c r="G71" s="35"/>
-      <c r="H71" s="35"/>
-      <c r="I71" s="35"/>
-      <c r="J71" s="35"/>
-      <c r="K71" s="35"/>
-      <c r="L71" s="34"/>
-      <c r="M71" s="44"/>
-      <c r="N71" s="44"/>
-      <c r="O71" s="44"/>
-      <c r="P71" s="44"/>
-      <c r="Q71" s="44"/>
-      <c r="R71" s="44"/>
-      <c r="S71" s="44"/>
-      <c r="T71" s="34"/>
-      <c r="U71" s="44"/>
-      <c r="V71" s="44"/>
-      <c r="W71" s="44"/>
-      <c r="X71" s="44"/>
-      <c r="Y71" s="44"/>
-      <c r="Z71" s="44"/>
-      <c r="AA71" s="44"/>
-      <c r="AB71" s="34"/>
-      <c r="AC71" s="44"/>
-      <c r="AD71" s="44"/>
-      <c r="AE71" s="44"/>
-      <c r="AF71" s="44"/>
-      <c r="AG71" s="44"/>
-      <c r="AH71" s="44"/>
-      <c r="AI71" s="44"/>
+      <c r="A71" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B71" s="62"/>
+      <c r="C71" s="14"/>
+      <c r="D71" s="5"/>
+      <c r="E71" s="4"/>
+      <c r="F71" s="4"/>
+      <c r="G71" s="4"/>
+      <c r="H71" s="4"/>
+      <c r="I71" s="4"/>
+      <c r="J71" s="4"/>
+      <c r="K71" s="4"/>
+      <c r="L71" s="5"/>
+      <c r="M71" s="42"/>
+      <c r="N71" s="42"/>
+      <c r="O71" s="42"/>
+      <c r="P71" s="42"/>
+      <c r="Q71" s="42"/>
+      <c r="R71" s="42"/>
+      <c r="S71" s="42"/>
+      <c r="T71" s="5"/>
+      <c r="U71" s="42"/>
+      <c r="V71" s="42"/>
+      <c r="W71" s="42"/>
+      <c r="X71" s="42"/>
+      <c r="Y71" s="42"/>
+      <c r="Z71" s="42"/>
+      <c r="AA71" s="42"/>
+      <c r="AB71" s="5"/>
+      <c r="AC71" s="42"/>
+      <c r="AD71" s="42"/>
+      <c r="AE71" s="42"/>
+      <c r="AF71" s="42"/>
+      <c r="AG71" s="42"/>
+      <c r="AH71" s="42"/>
+      <c r="AI71" s="42"/>
       <c r="AJ71" s="86"/>
       <c r="AK71" s="87"/>
       <c r="AL71" s="87"/>
@@ -27698,30 +27719,30 @@
       <c r="BE71" s="87"/>
       <c r="BF71" s="87"/>
       <c r="BG71" s="87"/>
-      <c r="BH71" s="34"/>
-      <c r="BI71" s="35"/>
-      <c r="BJ71" s="35"/>
-      <c r="BK71" s="35"/>
-      <c r="BL71" s="35"/>
-      <c r="BM71" s="35"/>
-      <c r="BN71" s="35"/>
-      <c r="BO71" s="35"/>
-      <c r="BP71" s="34"/>
-      <c r="BQ71" s="44"/>
-      <c r="BR71" s="44"/>
-      <c r="BS71" s="44"/>
-      <c r="BT71" s="44"/>
-      <c r="BU71" s="44"/>
-      <c r="BV71" s="44"/>
-      <c r="BW71" s="44"/>
-      <c r="BX71" s="34"/>
-      <c r="BY71" s="44"/>
-      <c r="BZ71" s="44"/>
-      <c r="CA71" s="44"/>
-      <c r="CB71" s="44"/>
-      <c r="CC71" s="44"/>
-      <c r="CD71" s="44"/>
-      <c r="CE71" s="44"/>
+      <c r="BH71" s="5"/>
+      <c r="BI71" s="4"/>
+      <c r="BJ71" s="4"/>
+      <c r="BK71" s="4"/>
+      <c r="BL71" s="4"/>
+      <c r="BM71" s="4"/>
+      <c r="BN71" s="4"/>
+      <c r="BO71" s="4"/>
+      <c r="BP71" s="5"/>
+      <c r="BQ71" s="42"/>
+      <c r="BR71" s="42"/>
+      <c r="BS71" s="42"/>
+      <c r="BT71" s="42"/>
+      <c r="BU71" s="42"/>
+      <c r="BV71" s="42"/>
+      <c r="BW71" s="42"/>
+      <c r="BX71" s="5"/>
+      <c r="BY71" s="42"/>
+      <c r="BZ71" s="42"/>
+      <c r="CA71" s="42"/>
+      <c r="CB71" s="42"/>
+      <c r="CC71" s="42"/>
+      <c r="CD71" s="42"/>
+      <c r="CE71" s="42"/>
       <c r="CF71" s="86"/>
       <c r="CG71" s="87"/>
       <c r="CH71" s="87"/>
@@ -27754,78 +27775,80 @@
       <c r="DI71" s="87"/>
       <c r="DJ71" s="87"/>
       <c r="DK71" s="87"/>
-      <c r="DL71" s="34"/>
-      <c r="DM71" s="44"/>
-      <c r="DN71" s="44"/>
-      <c r="DO71" s="44"/>
-      <c r="DP71" s="44"/>
-      <c r="DQ71" s="44"/>
-      <c r="DR71" s="44"/>
-      <c r="DS71" s="44"/>
-      <c r="DT71" s="34"/>
-      <c r="DU71" s="44"/>
-      <c r="DV71" s="44"/>
-      <c r="DW71" s="44"/>
-      <c r="DX71" s="44"/>
-      <c r="DY71" s="44"/>
-      <c r="DZ71" s="44"/>
-      <c r="EA71" s="44"/>
-      <c r="EB71" s="34"/>
-      <c r="EC71" s="35"/>
-      <c r="ED71" s="44"/>
-      <c r="EE71" s="44"/>
-      <c r="EF71" s="44"/>
-      <c r="EG71" s="44"/>
-      <c r="EH71" s="44"/>
-      <c r="EI71" s="44"/>
-      <c r="EJ71" s="34"/>
-      <c r="EK71" s="35"/>
-      <c r="EL71" s="44"/>
-      <c r="EM71" s="44"/>
-      <c r="EN71" s="44"/>
-      <c r="EO71" s="44"/>
-      <c r="EP71" s="44"/>
-      <c r="EQ71" s="72"/>
+      <c r="DL71" s="5"/>
+      <c r="DM71" s="42"/>
+      <c r="DN71" s="42"/>
+      <c r="DO71" s="42"/>
+      <c r="DP71" s="42"/>
+      <c r="DQ71" s="42"/>
+      <c r="DR71" s="42"/>
+      <c r="DS71" s="42"/>
+      <c r="DT71" s="5"/>
+      <c r="DU71" s="42"/>
+      <c r="DV71" s="42"/>
+      <c r="DW71" s="42"/>
+      <c r="DX71" s="42"/>
+      <c r="DY71" s="42"/>
+      <c r="DZ71" s="42"/>
+      <c r="EA71" s="42"/>
+      <c r="EB71" s="5"/>
+      <c r="EC71" s="4"/>
+      <c r="ED71" s="42"/>
+      <c r="EE71" s="42"/>
+      <c r="EF71" s="42"/>
+      <c r="EG71" s="42"/>
+      <c r="EH71" s="42"/>
+      <c r="EI71" s="42"/>
+      <c r="EJ71" s="5"/>
+      <c r="EK71" s="4"/>
+      <c r="EL71" s="42"/>
+      <c r="EM71" s="42"/>
+      <c r="EN71" s="42"/>
+      <c r="EO71" s="42"/>
+      <c r="EP71" s="42"/>
+      <c r="EQ71" s="70"/>
     </row>
-    <row r="72" spans="1:147" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="17"/>
-      <c r="B72" s="56"/>
-      <c r="C72" s="52" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="D72" s="36"/>
-      <c r="E72" s="37"/>
-      <c r="F72" s="37"/>
-      <c r="G72" s="37"/>
-      <c r="H72" s="37"/>
-      <c r="I72" s="37"/>
-      <c r="J72" s="37"/>
-      <c r="K72" s="37"/>
-      <c r="L72" s="36"/>
-      <c r="M72" s="45"/>
-      <c r="N72" s="45"/>
-      <c r="O72" s="45"/>
-      <c r="P72" s="45"/>
-      <c r="Q72" s="45"/>
-      <c r="R72" s="45"/>
-      <c r="S72" s="45"/>
-      <c r="T72" s="36"/>
-      <c r="U72" s="45"/>
-      <c r="V72" s="45"/>
-      <c r="W72" s="45"/>
-      <c r="X72" s="45"/>
-      <c r="Y72" s="45"/>
-      <c r="Z72" s="45"/>
-      <c r="AA72" s="45"/>
-      <c r="AB72" s="36"/>
-      <c r="AC72" s="45"/>
-      <c r="AD72" s="45"/>
-      <c r="AE72" s="45"/>
-      <c r="AF72" s="45"/>
-      <c r="AG72" s="45"/>
-      <c r="AH72" s="45"/>
-      <c r="AI72" s="45"/>
+    <row r="72" spans="1:147" x14ac:dyDescent="0.25">
+      <c r="A72" s="16"/>
+      <c r="B72" s="55" t="s">
+        <v>56</v>
+      </c>
+      <c r="C72" s="78">
+        <f t="shared" ref="C72:C82" si="6">IF($B72&gt;"",SUM(COUNTIF($D72:$EQ72,"R")),"")</f>
+        <v>0</v>
+      </c>
+      <c r="D72" s="75"/>
+      <c r="E72" s="76"/>
+      <c r="F72" s="76"/>
+      <c r="G72" s="76"/>
+      <c r="H72" s="76"/>
+      <c r="I72" s="76"/>
+      <c r="J72" s="76"/>
+      <c r="K72" s="76"/>
+      <c r="L72" s="77"/>
+      <c r="M72" s="75"/>
+      <c r="N72" s="75"/>
+      <c r="O72" s="75"/>
+      <c r="P72" s="75"/>
+      <c r="Q72" s="75"/>
+      <c r="R72" s="75"/>
+      <c r="S72" s="75"/>
+      <c r="T72" s="77"/>
+      <c r="U72" s="75"/>
+      <c r="V72" s="75"/>
+      <c r="W72" s="75"/>
+      <c r="X72" s="75"/>
+      <c r="Y72" s="75"/>
+      <c r="Z72" s="75"/>
+      <c r="AA72" s="75"/>
+      <c r="AB72" s="77"/>
+      <c r="AC72" s="75"/>
+      <c r="AD72" s="75"/>
+      <c r="AE72" s="75"/>
+      <c r="AF72" s="75"/>
+      <c r="AG72" s="75"/>
+      <c r="AH72" s="75"/>
+      <c r="AI72" s="75"/>
       <c r="AJ72" s="86"/>
       <c r="AK72" s="87"/>
       <c r="AL72" s="87"/>
@@ -27850,30 +27873,30 @@
       <c r="BE72" s="87"/>
       <c r="BF72" s="87"/>
       <c r="BG72" s="87"/>
-      <c r="BH72" s="36"/>
-      <c r="BI72" s="37"/>
-      <c r="BJ72" s="37"/>
-      <c r="BK72" s="37"/>
-      <c r="BL72" s="37"/>
-      <c r="BM72" s="37"/>
-      <c r="BN72" s="37"/>
-      <c r="BO72" s="37"/>
-      <c r="BP72" s="36"/>
-      <c r="BQ72" s="45"/>
-      <c r="BR72" s="45"/>
-      <c r="BS72" s="45"/>
-      <c r="BT72" s="45"/>
-      <c r="BU72" s="45"/>
-      <c r="BV72" s="45"/>
-      <c r="BW72" s="45"/>
-      <c r="BX72" s="36"/>
-      <c r="BY72" s="45"/>
-      <c r="BZ72" s="45"/>
-      <c r="CA72" s="45"/>
-      <c r="CB72" s="45"/>
-      <c r="CC72" s="45"/>
-      <c r="CD72" s="45"/>
-      <c r="CE72" s="45"/>
+      <c r="BH72" s="79"/>
+      <c r="BI72" s="76"/>
+      <c r="BJ72" s="76"/>
+      <c r="BK72" s="76"/>
+      <c r="BL72" s="76"/>
+      <c r="BM72" s="76"/>
+      <c r="BN72" s="76"/>
+      <c r="BO72" s="76"/>
+      <c r="BP72" s="77"/>
+      <c r="BQ72" s="75"/>
+      <c r="BR72" s="75"/>
+      <c r="BS72" s="75"/>
+      <c r="BT72" s="75"/>
+      <c r="BU72" s="75"/>
+      <c r="BV72" s="75"/>
+      <c r="BW72" s="75"/>
+      <c r="BX72" s="77"/>
+      <c r="BY72" s="75"/>
+      <c r="BZ72" s="75"/>
+      <c r="CA72" s="75"/>
+      <c r="CB72" s="75"/>
+      <c r="CC72" s="75"/>
+      <c r="CD72" s="75"/>
+      <c r="CE72" s="75"/>
       <c r="CF72" s="86"/>
       <c r="CG72" s="87"/>
       <c r="CH72" s="87"/>
@@ -27906,77 +27929,80 @@
       <c r="DI72" s="87"/>
       <c r="DJ72" s="87"/>
       <c r="DK72" s="87"/>
-      <c r="DL72" s="36"/>
-      <c r="DM72" s="45"/>
-      <c r="DN72" s="45"/>
-      <c r="DO72" s="45"/>
-      <c r="DP72" s="45"/>
-      <c r="DQ72" s="45"/>
-      <c r="DR72" s="45"/>
-      <c r="DS72" s="45"/>
-      <c r="DT72" s="36"/>
-      <c r="DU72" s="45"/>
-      <c r="DV72" s="45"/>
-      <c r="DW72" s="45"/>
-      <c r="DX72" s="45"/>
-      <c r="DY72" s="45"/>
-      <c r="DZ72" s="45"/>
-      <c r="EA72" s="45"/>
-      <c r="EB72" s="36"/>
-      <c r="EC72" s="37"/>
-      <c r="ED72" s="45"/>
-      <c r="EE72" s="45"/>
-      <c r="EF72" s="45"/>
-      <c r="EG72" s="45"/>
-      <c r="EH72" s="45"/>
-      <c r="EI72" s="45"/>
-      <c r="EJ72" s="36"/>
-      <c r="EK72" s="37"/>
-      <c r="EL72" s="45"/>
-      <c r="EM72" s="45"/>
-      <c r="EN72" s="45"/>
-      <c r="EO72" s="45"/>
-      <c r="EP72" s="45"/>
-      <c r="EQ72" s="73"/>
+      <c r="DL72" s="77"/>
+      <c r="DM72" s="75"/>
+      <c r="DN72" s="75"/>
+      <c r="DO72" s="75"/>
+      <c r="DP72" s="75"/>
+      <c r="DQ72" s="75"/>
+      <c r="DR72" s="75"/>
+      <c r="DS72" s="75"/>
+      <c r="DT72" s="77"/>
+      <c r="DU72" s="75"/>
+      <c r="DV72" s="75"/>
+      <c r="DW72" s="75"/>
+      <c r="DX72" s="75"/>
+      <c r="DY72" s="75"/>
+      <c r="DZ72" s="75"/>
+      <c r="EA72" s="75"/>
+      <c r="EB72" s="32"/>
+      <c r="EC72" s="33"/>
+      <c r="ED72" s="33"/>
+      <c r="EE72" s="33"/>
+      <c r="EF72" s="33"/>
+      <c r="EG72" s="33"/>
+      <c r="EH72" s="33"/>
+      <c r="EI72" s="33"/>
+      <c r="EJ72" s="32"/>
+      <c r="EK72" s="33"/>
+      <c r="EL72" s="33"/>
+      <c r="EM72" s="33"/>
+      <c r="EN72" s="33"/>
+      <c r="EO72" s="33"/>
+      <c r="EP72" s="33"/>
+      <c r="EQ72" s="33"/>
     </row>
     <row r="73" spans="1:147" x14ac:dyDescent="0.25">
-      <c r="A73" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="B73" s="62"/>
-      <c r="C73" s="14"/>
-      <c r="D73" s="5"/>
-      <c r="E73" s="4"/>
-      <c r="F73" s="4"/>
-      <c r="G73" s="4"/>
-      <c r="H73" s="4"/>
-      <c r="I73" s="4"/>
-      <c r="J73" s="4"/>
-      <c r="K73" s="4"/>
-      <c r="L73" s="5"/>
-      <c r="M73" s="42"/>
-      <c r="N73" s="42"/>
-      <c r="O73" s="42"/>
-      <c r="P73" s="42"/>
-      <c r="Q73" s="42"/>
-      <c r="R73" s="42"/>
-      <c r="S73" s="42"/>
-      <c r="T73" s="5"/>
-      <c r="U73" s="42"/>
-      <c r="V73" s="42"/>
-      <c r="W73" s="42"/>
-      <c r="X73" s="42"/>
-      <c r="Y73" s="42"/>
-      <c r="Z73" s="42"/>
-      <c r="AA73" s="42"/>
-      <c r="AB73" s="5"/>
-      <c r="AC73" s="42"/>
-      <c r="AD73" s="42"/>
-      <c r="AE73" s="42"/>
-      <c r="AF73" s="42"/>
-      <c r="AG73" s="42"/>
-      <c r="AH73" s="42"/>
-      <c r="AI73" s="42"/>
+      <c r="A73" s="16"/>
+      <c r="B73" s="55" t="s">
+        <v>49</v>
+      </c>
+      <c r="C73" s="9">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="D73" s="38"/>
+      <c r="E73" s="33"/>
+      <c r="F73" s="33"/>
+      <c r="G73" s="33"/>
+      <c r="H73" s="33"/>
+      <c r="I73" s="33"/>
+      <c r="J73" s="33"/>
+      <c r="K73" s="33"/>
+      <c r="L73" s="32"/>
+      <c r="M73" s="43"/>
+      <c r="N73" s="43"/>
+      <c r="O73" s="43"/>
+      <c r="P73" s="43"/>
+      <c r="Q73" s="43"/>
+      <c r="R73" s="43"/>
+      <c r="S73" s="43"/>
+      <c r="T73" s="32"/>
+      <c r="U73" s="43"/>
+      <c r="V73" s="43"/>
+      <c r="W73" s="43"/>
+      <c r="X73" s="43"/>
+      <c r="Y73" s="43"/>
+      <c r="Z73" s="43"/>
+      <c r="AA73" s="43"/>
+      <c r="AB73" s="32"/>
+      <c r="AC73" s="43"/>
+      <c r="AD73" s="43"/>
+      <c r="AE73" s="43"/>
+      <c r="AF73" s="43"/>
+      <c r="AG73" s="43"/>
+      <c r="AH73" s="43"/>
+      <c r="AI73" s="43"/>
       <c r="AJ73" s="86"/>
       <c r="AK73" s="87"/>
       <c r="AL73" s="87"/>
@@ -28001,30 +28027,30 @@
       <c r="BE73" s="87"/>
       <c r="BF73" s="87"/>
       <c r="BG73" s="87"/>
-      <c r="BH73" s="5"/>
-      <c r="BI73" s="4"/>
-      <c r="BJ73" s="4"/>
-      <c r="BK73" s="4"/>
-      <c r="BL73" s="4"/>
-      <c r="BM73" s="4"/>
-      <c r="BN73" s="4"/>
-      <c r="BO73" s="4"/>
-      <c r="BP73" s="5"/>
-      <c r="BQ73" s="42"/>
-      <c r="BR73" s="42"/>
-      <c r="BS73" s="42"/>
-      <c r="BT73" s="42"/>
-      <c r="BU73" s="42"/>
-      <c r="BV73" s="42"/>
-      <c r="BW73" s="42"/>
-      <c r="BX73" s="5"/>
-      <c r="BY73" s="42"/>
-      <c r="BZ73" s="42"/>
-      <c r="CA73" s="42"/>
-      <c r="CB73" s="42"/>
-      <c r="CC73" s="42"/>
-      <c r="CD73" s="42"/>
-      <c r="CE73" s="42"/>
+      <c r="BH73" s="38"/>
+      <c r="BI73" s="33"/>
+      <c r="BJ73" s="33"/>
+      <c r="BK73" s="33"/>
+      <c r="BL73" s="33"/>
+      <c r="BM73" s="33"/>
+      <c r="BN73" s="33"/>
+      <c r="BO73" s="33"/>
+      <c r="BP73" s="32"/>
+      <c r="BQ73" s="43"/>
+      <c r="BR73" s="43"/>
+      <c r="BS73" s="43"/>
+      <c r="BT73" s="43"/>
+      <c r="BU73" s="43"/>
+      <c r="BV73" s="43"/>
+      <c r="BW73" s="43"/>
+      <c r="BX73" s="32"/>
+      <c r="BY73" s="43"/>
+      <c r="BZ73" s="43"/>
+      <c r="CA73" s="43"/>
+      <c r="CB73" s="43"/>
+      <c r="CC73" s="43"/>
+      <c r="CD73" s="43"/>
+      <c r="CE73" s="43"/>
       <c r="CF73" s="86"/>
       <c r="CG73" s="87"/>
       <c r="CH73" s="87"/>
@@ -28057,80 +28083,80 @@
       <c r="DI73" s="87"/>
       <c r="DJ73" s="87"/>
       <c r="DK73" s="87"/>
-      <c r="DL73" s="5"/>
-      <c r="DM73" s="42"/>
-      <c r="DN73" s="42"/>
-      <c r="DO73" s="42"/>
-      <c r="DP73" s="42"/>
-      <c r="DQ73" s="42"/>
-      <c r="DR73" s="42"/>
-      <c r="DS73" s="42"/>
-      <c r="DT73" s="5"/>
-      <c r="DU73" s="42"/>
-      <c r="DV73" s="42"/>
-      <c r="DW73" s="42"/>
-      <c r="DX73" s="42"/>
-      <c r="DY73" s="42"/>
-      <c r="DZ73" s="42"/>
-      <c r="EA73" s="42"/>
-      <c r="EB73" s="5"/>
-      <c r="EC73" s="4"/>
-      <c r="ED73" s="42"/>
-      <c r="EE73" s="42"/>
-      <c r="EF73" s="42"/>
-      <c r="EG73" s="42"/>
-      <c r="EH73" s="42"/>
-      <c r="EI73" s="42"/>
-      <c r="EJ73" s="5"/>
-      <c r="EK73" s="4"/>
-      <c r="EL73" s="42"/>
-      <c r="EM73" s="42"/>
-      <c r="EN73" s="42"/>
-      <c r="EO73" s="42"/>
-      <c r="EP73" s="42"/>
-      <c r="EQ73" s="70"/>
+      <c r="DL73" s="32"/>
+      <c r="DM73" s="43"/>
+      <c r="DN73" s="43"/>
+      <c r="DO73" s="43"/>
+      <c r="DP73" s="43"/>
+      <c r="DQ73" s="43"/>
+      <c r="DR73" s="43"/>
+      <c r="DS73" s="43"/>
+      <c r="DT73" s="32"/>
+      <c r="DU73" s="43"/>
+      <c r="DV73" s="43"/>
+      <c r="DW73" s="43"/>
+      <c r="DX73" s="43"/>
+      <c r="DY73" s="43"/>
+      <c r="DZ73" s="43"/>
+      <c r="EA73" s="43"/>
+      <c r="EB73" s="32"/>
+      <c r="EC73" s="33"/>
+      <c r="ED73" s="33"/>
+      <c r="EE73" s="33"/>
+      <c r="EF73" s="33"/>
+      <c r="EG73" s="33"/>
+      <c r="EH73" s="33"/>
+      <c r="EI73" s="33"/>
+      <c r="EJ73" s="32"/>
+      <c r="EK73" s="33"/>
+      <c r="EL73" s="33"/>
+      <c r="EM73" s="33"/>
+      <c r="EN73" s="33"/>
+      <c r="EO73" s="33"/>
+      <c r="EP73" s="33"/>
+      <c r="EQ73" s="33"/>
     </row>
     <row r="74" spans="1:147" x14ac:dyDescent="0.25">
       <c r="A74" s="16"/>
       <c r="B74" s="55" t="s">
-        <v>56</v>
-      </c>
-      <c r="C74" s="78">
-        <f t="shared" ref="C74:C84" si="6">IF($B74&gt;"",SUM(COUNTIF($D74:$EQ74,"R")),"")</f>
+        <v>50</v>
+      </c>
+      <c r="C74" s="9">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="D74" s="75"/>
-      <c r="E74" s="76"/>
-      <c r="F74" s="76"/>
-      <c r="G74" s="76"/>
-      <c r="H74" s="76"/>
-      <c r="I74" s="76"/>
-      <c r="J74" s="76"/>
-      <c r="K74" s="76"/>
-      <c r="L74" s="77"/>
-      <c r="M74" s="75"/>
-      <c r="N74" s="75"/>
-      <c r="O74" s="75"/>
-      <c r="P74" s="75"/>
-      <c r="Q74" s="75"/>
-      <c r="R74" s="75"/>
-      <c r="S74" s="75"/>
-      <c r="T74" s="77"/>
-      <c r="U74" s="75"/>
-      <c r="V74" s="75"/>
-      <c r="W74" s="75"/>
-      <c r="X74" s="75"/>
-      <c r="Y74" s="75"/>
-      <c r="Z74" s="75"/>
-      <c r="AA74" s="75"/>
-      <c r="AB74" s="77"/>
-      <c r="AC74" s="75"/>
-      <c r="AD74" s="75"/>
-      <c r="AE74" s="75"/>
-      <c r="AF74" s="75"/>
-      <c r="AG74" s="75"/>
-      <c r="AH74" s="75"/>
-      <c r="AI74" s="75"/>
+      <c r="D74" s="39"/>
+      <c r="E74" s="35"/>
+      <c r="F74" s="35"/>
+      <c r="G74" s="35"/>
+      <c r="H74" s="35"/>
+      <c r="I74" s="35"/>
+      <c r="J74" s="35"/>
+      <c r="K74" s="35"/>
+      <c r="L74" s="34"/>
+      <c r="M74" s="44"/>
+      <c r="N74" s="44"/>
+      <c r="O74" s="44"/>
+      <c r="P74" s="44"/>
+      <c r="Q74" s="44"/>
+      <c r="R74" s="44"/>
+      <c r="S74" s="44"/>
+      <c r="T74" s="34"/>
+      <c r="U74" s="44"/>
+      <c r="V74" s="44"/>
+      <c r="W74" s="44"/>
+      <c r="X74" s="44"/>
+      <c r="Y74" s="44"/>
+      <c r="Z74" s="44"/>
+      <c r="AA74" s="44"/>
+      <c r="AB74" s="34"/>
+      <c r="AC74" s="44"/>
+      <c r="AD74" s="44"/>
+      <c r="AE74" s="44"/>
+      <c r="AF74" s="44"/>
+      <c r="AG74" s="44"/>
+      <c r="AH74" s="44"/>
+      <c r="AI74" s="44"/>
       <c r="AJ74" s="86"/>
       <c r="AK74" s="87"/>
       <c r="AL74" s="87"/>
@@ -28155,30 +28181,30 @@
       <c r="BE74" s="87"/>
       <c r="BF74" s="87"/>
       <c r="BG74" s="87"/>
-      <c r="BH74" s="79"/>
-      <c r="BI74" s="76"/>
-      <c r="BJ74" s="76"/>
-      <c r="BK74" s="76"/>
-      <c r="BL74" s="76"/>
-      <c r="BM74" s="76"/>
-      <c r="BN74" s="76"/>
-      <c r="BO74" s="76"/>
-      <c r="BP74" s="77"/>
-      <c r="BQ74" s="75"/>
-      <c r="BR74" s="75"/>
-      <c r="BS74" s="75"/>
-      <c r="BT74" s="75"/>
-      <c r="BU74" s="75"/>
-      <c r="BV74" s="75"/>
-      <c r="BW74" s="75"/>
-      <c r="BX74" s="77"/>
-      <c r="BY74" s="75"/>
-      <c r="BZ74" s="75"/>
-      <c r="CA74" s="75"/>
-      <c r="CB74" s="75"/>
-      <c r="CC74" s="75"/>
-      <c r="CD74" s="75"/>
-      <c r="CE74" s="75"/>
+      <c r="BH74" s="39"/>
+      <c r="BI74" s="35"/>
+      <c r="BJ74" s="35"/>
+      <c r="BK74" s="35"/>
+      <c r="BL74" s="35"/>
+      <c r="BM74" s="35"/>
+      <c r="BN74" s="35"/>
+      <c r="BO74" s="35"/>
+      <c r="BP74" s="34"/>
+      <c r="BQ74" s="44"/>
+      <c r="BR74" s="44"/>
+      <c r="BS74" s="44"/>
+      <c r="BT74" s="44"/>
+      <c r="BU74" s="44"/>
+      <c r="BV74" s="44"/>
+      <c r="BW74" s="44"/>
+      <c r="BX74" s="34"/>
+      <c r="BY74" s="44"/>
+      <c r="BZ74" s="44"/>
+      <c r="CA74" s="44"/>
+      <c r="CB74" s="44"/>
+      <c r="CC74" s="44"/>
+      <c r="CD74" s="44"/>
+      <c r="CE74" s="44"/>
       <c r="CF74" s="86"/>
       <c r="CG74" s="87"/>
       <c r="CH74" s="87"/>
@@ -28211,22 +28237,22 @@
       <c r="DI74" s="87"/>
       <c r="DJ74" s="87"/>
       <c r="DK74" s="87"/>
-      <c r="DL74" s="77"/>
-      <c r="DM74" s="75"/>
-      <c r="DN74" s="75"/>
-      <c r="DO74" s="75"/>
-      <c r="DP74" s="75"/>
-      <c r="DQ74" s="75"/>
-      <c r="DR74" s="75"/>
-      <c r="DS74" s="75"/>
-      <c r="DT74" s="77"/>
-      <c r="DU74" s="75"/>
-      <c r="DV74" s="75"/>
-      <c r="DW74" s="75"/>
-      <c r="DX74" s="75"/>
-      <c r="DY74" s="75"/>
-      <c r="DZ74" s="75"/>
-      <c r="EA74" s="75"/>
+      <c r="DL74" s="34"/>
+      <c r="DM74" s="44"/>
+      <c r="DN74" s="44"/>
+      <c r="DO74" s="44"/>
+      <c r="DP74" s="44"/>
+      <c r="DQ74" s="44"/>
+      <c r="DR74" s="44"/>
+      <c r="DS74" s="44"/>
+      <c r="DT74" s="34"/>
+      <c r="DU74" s="44"/>
+      <c r="DV74" s="44"/>
+      <c r="DW74" s="44"/>
+      <c r="DX74" s="44"/>
+      <c r="DY74" s="44"/>
+      <c r="DZ74" s="44"/>
+      <c r="EA74" s="44"/>
       <c r="EB74" s="32"/>
       <c r="EC74" s="33"/>
       <c r="ED74" s="33"/>
@@ -28247,44 +28273,108 @@
     <row r="75" spans="1:147" x14ac:dyDescent="0.25">
       <c r="A75" s="16"/>
       <c r="B75" s="55" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="C75" s="9">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="D75" s="38"/>
-      <c r="E75" s="33"/>
-      <c r="F75" s="33"/>
-      <c r="G75" s="33"/>
-      <c r="H75" s="33"/>
-      <c r="I75" s="33"/>
-      <c r="J75" s="33"/>
-      <c r="K75" s="33"/>
-      <c r="L75" s="32"/>
-      <c r="M75" s="43"/>
-      <c r="N75" s="43"/>
-      <c r="O75" s="43"/>
-      <c r="P75" s="43"/>
-      <c r="Q75" s="43"/>
-      <c r="R75" s="43"/>
-      <c r="S75" s="43"/>
-      <c r="T75" s="32"/>
-      <c r="U75" s="43"/>
-      <c r="V75" s="43"/>
-      <c r="W75" s="43"/>
-      <c r="X75" s="43"/>
-      <c r="Y75" s="43"/>
-      <c r="Z75" s="43"/>
-      <c r="AA75" s="43"/>
-      <c r="AB75" s="32"/>
-      <c r="AC75" s="43"/>
-      <c r="AD75" s="43"/>
-      <c r="AE75" s="43"/>
-      <c r="AF75" s="43"/>
-      <c r="AG75" s="43"/>
-      <c r="AH75" s="43"/>
-      <c r="AI75" s="43"/>
+      <c r="D75" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="E75" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="F75" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="G75" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="H75" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="I75" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="J75" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="K75" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="L75" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="M75" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="N75" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="O75" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="P75" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q75" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="R75" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="S75" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="T75" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="U75" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="V75" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="W75" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="X75" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y75" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z75" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA75" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB75" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="AC75" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="AD75" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE75" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF75" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="AG75" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="AH75" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="AI75" s="35" t="s">
+        <v>12</v>
+      </c>
       <c r="AJ75" s="86"/>
       <c r="AK75" s="87"/>
       <c r="AL75" s="87"/>
@@ -28309,30 +28399,78 @@
       <c r="BE75" s="87"/>
       <c r="BF75" s="87"/>
       <c r="BG75" s="87"/>
-      <c r="BH75" s="38"/>
-      <c r="BI75" s="33"/>
-      <c r="BJ75" s="33"/>
-      <c r="BK75" s="33"/>
-      <c r="BL75" s="33"/>
-      <c r="BM75" s="33"/>
-      <c r="BN75" s="33"/>
-      <c r="BO75" s="33"/>
-      <c r="BP75" s="32"/>
-      <c r="BQ75" s="43"/>
-      <c r="BR75" s="43"/>
-      <c r="BS75" s="43"/>
-      <c r="BT75" s="43"/>
-      <c r="BU75" s="43"/>
-      <c r="BV75" s="43"/>
-      <c r="BW75" s="43"/>
-      <c r="BX75" s="32"/>
-      <c r="BY75" s="43"/>
-      <c r="BZ75" s="43"/>
-      <c r="CA75" s="43"/>
-      <c r="CB75" s="43"/>
-      <c r="CC75" s="43"/>
-      <c r="CD75" s="43"/>
-      <c r="CE75" s="43"/>
+      <c r="BH75" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="BI75" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="BJ75" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="BK75" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="BL75" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="BM75" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="BN75" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="BO75" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="BP75" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="BQ75" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="BR75" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="BS75" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="BT75" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="BU75" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="BV75" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="BW75" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="BX75" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="BY75" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="BZ75" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="CA75" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="CB75" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="CC75" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="CD75" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="CE75" s="35" t="s">
+        <v>12</v>
+      </c>
       <c r="CF75" s="86"/>
       <c r="CG75" s="87"/>
       <c r="CH75" s="87"/>
@@ -28365,47 +28503,109 @@
       <c r="DI75" s="87"/>
       <c r="DJ75" s="87"/>
       <c r="DK75" s="87"/>
-      <c r="DL75" s="32"/>
-      <c r="DM75" s="43"/>
-      <c r="DN75" s="43"/>
-      <c r="DO75" s="43"/>
-      <c r="DP75" s="43"/>
-      <c r="DQ75" s="43"/>
-      <c r="DR75" s="43"/>
-      <c r="DS75" s="43"/>
-      <c r="DT75" s="32"/>
-      <c r="DU75" s="43"/>
-      <c r="DV75" s="43"/>
-      <c r="DW75" s="43"/>
-      <c r="DX75" s="43"/>
-      <c r="DY75" s="43"/>
-      <c r="DZ75" s="43"/>
-      <c r="EA75" s="43"/>
-      <c r="EB75" s="32"/>
-      <c r="EC75" s="33"/>
-      <c r="ED75" s="33"/>
-      <c r="EE75" s="33"/>
-      <c r="EF75" s="33"/>
-      <c r="EG75" s="33"/>
-      <c r="EH75" s="33"/>
-      <c r="EI75" s="33"/>
-      <c r="EJ75" s="32"/>
-      <c r="EK75" s="33"/>
-      <c r="EL75" s="33"/>
-      <c r="EM75" s="33"/>
-      <c r="EN75" s="33"/>
-      <c r="EO75" s="33"/>
-      <c r="EP75" s="33"/>
-      <c r="EQ75" s="33"/>
+      <c r="DL75" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="DM75" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="DN75" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="DO75" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="DP75" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="DQ75" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="DR75" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="DS75" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="DT75" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="DU75" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="DV75" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="DW75" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="DX75" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="DY75" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="DZ75" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="EA75" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="EB75" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="EC75" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="ED75" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="EE75" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="EF75" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="EG75" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="EH75" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="EI75" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="EJ75" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="EK75" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="EL75" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="EM75" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="EN75" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="EO75" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="EP75" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="EQ75" s="35" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="76" spans="1:147" x14ac:dyDescent="0.25">
       <c r="A76" s="16"/>
-      <c r="B76" s="55" t="s">
-        <v>50</v>
-      </c>
-      <c r="C76" s="9">
+      <c r="B76" s="55"/>
+      <c r="C76" s="9" t="str">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="D76" s="39"/>
       <c r="E76" s="35"/>
@@ -28535,128 +28735,62 @@
       <c r="DY76" s="44"/>
       <c r="DZ76" s="44"/>
       <c r="EA76" s="44"/>
-      <c r="EB76" s="32"/>
-      <c r="EC76" s="33"/>
-      <c r="ED76" s="33"/>
-      <c r="EE76" s="33"/>
-      <c r="EF76" s="33"/>
-      <c r="EG76" s="33"/>
-      <c r="EH76" s="33"/>
-      <c r="EI76" s="33"/>
-      <c r="EJ76" s="32"/>
-      <c r="EK76" s="33"/>
-      <c r="EL76" s="33"/>
-      <c r="EM76" s="33"/>
-      <c r="EN76" s="33"/>
-      <c r="EO76" s="33"/>
-      <c r="EP76" s="33"/>
-      <c r="EQ76" s="33"/>
+      <c r="EB76" s="34"/>
+      <c r="EC76" s="35"/>
+      <c r="ED76" s="44"/>
+      <c r="EE76" s="44"/>
+      <c r="EF76" s="44"/>
+      <c r="EG76" s="44"/>
+      <c r="EH76" s="44"/>
+      <c r="EI76" s="44"/>
+      <c r="EJ76" s="34"/>
+      <c r="EK76" s="35"/>
+      <c r="EL76" s="44"/>
+      <c r="EM76" s="44"/>
+      <c r="EN76" s="44"/>
+      <c r="EO76" s="44"/>
+      <c r="EP76" s="44"/>
+      <c r="EQ76" s="72"/>
     </row>
     <row r="77" spans="1:147" x14ac:dyDescent="0.25">
       <c r="A77" s="16"/>
-      <c r="B77" s="55" t="s">
-        <v>40</v>
-      </c>
-      <c r="C77" s="9">
+      <c r="B77" s="55"/>
+      <c r="C77" s="9" t="str">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="D77" s="39" t="s">
-        <v>12</v>
-      </c>
-      <c r="E77" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="F77" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="G77" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="H77" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="I77" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="J77" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="K77" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="L77" s="39" t="s">
-        <v>12</v>
-      </c>
-      <c r="M77" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="N77" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="O77" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="P77" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q77" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="R77" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="S77" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="T77" s="39" t="s">
-        <v>12</v>
-      </c>
-      <c r="U77" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="V77" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="W77" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="X77" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="Y77" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="Z77" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="AA77" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="AB77" s="39" t="s">
-        <v>12</v>
-      </c>
-      <c r="AC77" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="AD77" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="AE77" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="AF77" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="AG77" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="AH77" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="AI77" s="35" t="s">
-        <v>12</v>
-      </c>
+        <v/>
+      </c>
+      <c r="D77" s="39"/>
+      <c r="E77" s="35"/>
+      <c r="F77" s="35"/>
+      <c r="G77" s="35"/>
+      <c r="H77" s="35"/>
+      <c r="I77" s="35"/>
+      <c r="J77" s="35"/>
+      <c r="K77" s="35"/>
+      <c r="L77" s="34"/>
+      <c r="M77" s="44"/>
+      <c r="N77" s="44"/>
+      <c r="O77" s="44"/>
+      <c r="P77" s="44"/>
+      <c r="Q77" s="44"/>
+      <c r="R77" s="44"/>
+      <c r="S77" s="44"/>
+      <c r="T77" s="34"/>
+      <c r="U77" s="44"/>
+      <c r="V77" s="44"/>
+      <c r="W77" s="44"/>
+      <c r="X77" s="44"/>
+      <c r="Y77" s="44"/>
+      <c r="Z77" s="44"/>
+      <c r="AA77" s="44"/>
+      <c r="AB77" s="34"/>
+      <c r="AC77" s="44"/>
+      <c r="AD77" s="44"/>
+      <c r="AE77" s="44"/>
+      <c r="AF77" s="44"/>
+      <c r="AG77" s="44"/>
+      <c r="AH77" s="44"/>
+      <c r="AI77" s="44"/>
       <c r="AJ77" s="86"/>
       <c r="AK77" s="87"/>
       <c r="AL77" s="87"/>
@@ -28681,78 +28815,30 @@
       <c r="BE77" s="87"/>
       <c r="BF77" s="87"/>
       <c r="BG77" s="87"/>
-      <c r="BH77" s="39" t="s">
-        <v>12</v>
-      </c>
-      <c r="BI77" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="BJ77" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="BK77" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="BL77" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="BM77" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="BN77" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="BO77" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="BP77" s="39" t="s">
-        <v>12</v>
-      </c>
-      <c r="BQ77" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="BR77" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="BS77" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="BT77" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="BU77" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="BV77" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="BW77" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="BX77" s="39" t="s">
-        <v>12</v>
-      </c>
-      <c r="BY77" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="BZ77" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="CA77" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="CB77" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="CC77" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="CD77" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="CE77" s="35" t="s">
-        <v>12</v>
-      </c>
+      <c r="BH77" s="39"/>
+      <c r="BI77" s="35"/>
+      <c r="BJ77" s="35"/>
+      <c r="BK77" s="35"/>
+      <c r="BL77" s="35"/>
+      <c r="BM77" s="35"/>
+      <c r="BN77" s="35"/>
+      <c r="BO77" s="35"/>
+      <c r="BP77" s="34"/>
+      <c r="BQ77" s="44"/>
+      <c r="BR77" s="44"/>
+      <c r="BS77" s="44"/>
+      <c r="BT77" s="44"/>
+      <c r="BU77" s="44"/>
+      <c r="BV77" s="44"/>
+      <c r="BW77" s="44"/>
+      <c r="BX77" s="34"/>
+      <c r="BY77" s="44"/>
+      <c r="BZ77" s="44"/>
+      <c r="CA77" s="44"/>
+      <c r="CB77" s="44"/>
+      <c r="CC77" s="44"/>
+      <c r="CD77" s="44"/>
+      <c r="CE77" s="44"/>
       <c r="CF77" s="86"/>
       <c r="CG77" s="87"/>
       <c r="CH77" s="87"/>
@@ -28785,102 +28871,38 @@
       <c r="DI77" s="87"/>
       <c r="DJ77" s="87"/>
       <c r="DK77" s="87"/>
-      <c r="DL77" s="39" t="s">
-        <v>12</v>
-      </c>
-      <c r="DM77" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="DN77" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="DO77" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="DP77" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="DQ77" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="DR77" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="DS77" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="DT77" s="39" t="s">
-        <v>12</v>
-      </c>
-      <c r="DU77" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="DV77" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="DW77" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="DX77" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="DY77" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="DZ77" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="EA77" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="EB77" s="39" t="s">
-        <v>12</v>
-      </c>
-      <c r="EC77" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="ED77" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="EE77" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="EF77" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="EG77" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="EH77" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="EI77" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="EJ77" s="39" t="s">
-        <v>12</v>
-      </c>
-      <c r="EK77" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="EL77" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="EM77" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="EN77" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="EO77" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="EP77" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="EQ77" s="35" t="s">
-        <v>12</v>
-      </c>
+      <c r="DL77" s="34"/>
+      <c r="DM77" s="44"/>
+      <c r="DN77" s="44"/>
+      <c r="DO77" s="44"/>
+      <c r="DP77" s="44"/>
+      <c r="DQ77" s="44"/>
+      <c r="DR77" s="44"/>
+      <c r="DS77" s="44"/>
+      <c r="DT77" s="34"/>
+      <c r="DU77" s="44"/>
+      <c r="DV77" s="44"/>
+      <c r="DW77" s="44"/>
+      <c r="DX77" s="44"/>
+      <c r="DY77" s="44"/>
+      <c r="DZ77" s="44"/>
+      <c r="EA77" s="44"/>
+      <c r="EB77" s="34"/>
+      <c r="EC77" s="35"/>
+      <c r="ED77" s="44"/>
+      <c r="EE77" s="44"/>
+      <c r="EF77" s="44"/>
+      <c r="EG77" s="44"/>
+      <c r="EH77" s="44"/>
+      <c r="EI77" s="44"/>
+      <c r="EJ77" s="34"/>
+      <c r="EK77" s="35"/>
+      <c r="EL77" s="44"/>
+      <c r="EM77" s="44"/>
+      <c r="EN77" s="44"/>
+      <c r="EO77" s="44"/>
+      <c r="EP77" s="44"/>
+      <c r="EQ77" s="72"/>
     </row>
     <row r="78" spans="1:147" x14ac:dyDescent="0.25">
       <c r="A78" s="16"/>
@@ -29490,484 +29512,180 @@
       <c r="EP81" s="44"/>
       <c r="EQ81" s="72"/>
     </row>
-    <row r="82" spans="1:147" x14ac:dyDescent="0.25">
-      <c r="A82" s="16"/>
-      <c r="B82" s="55"/>
-      <c r="C82" s="9" t="str">
+    <row r="82" spans="1:147" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="17"/>
+      <c r="B82" s="56"/>
+      <c r="C82" s="53" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="D82" s="39"/>
-      <c r="E82" s="35"/>
-      <c r="F82" s="35"/>
-      <c r="G82" s="35"/>
-      <c r="H82" s="35"/>
-      <c r="I82" s="35"/>
-      <c r="J82" s="35"/>
-      <c r="K82" s="35"/>
-      <c r="L82" s="34"/>
-      <c r="M82" s="44"/>
-      <c r="N82" s="44"/>
-      <c r="O82" s="44"/>
-      <c r="P82" s="44"/>
-      <c r="Q82" s="44"/>
-      <c r="R82" s="44"/>
-      <c r="S82" s="44"/>
-      <c r="T82" s="34"/>
-      <c r="U82" s="44"/>
-      <c r="V82" s="44"/>
-      <c r="W82" s="44"/>
-      <c r="X82" s="44"/>
-      <c r="Y82" s="44"/>
-      <c r="Z82" s="44"/>
-      <c r="AA82" s="44"/>
-      <c r="AB82" s="34"/>
-      <c r="AC82" s="44"/>
-      <c r="AD82" s="44"/>
-      <c r="AE82" s="44"/>
-      <c r="AF82" s="44"/>
-      <c r="AG82" s="44"/>
-      <c r="AH82" s="44"/>
-      <c r="AI82" s="44"/>
-      <c r="AJ82" s="86"/>
-      <c r="AK82" s="87"/>
-      <c r="AL82" s="87"/>
-      <c r="AM82" s="87"/>
-      <c r="AN82" s="87"/>
-      <c r="AO82" s="87"/>
-      <c r="AP82" s="87"/>
-      <c r="AQ82" s="87"/>
-      <c r="AR82" s="86"/>
-      <c r="AS82" s="87"/>
-      <c r="AT82" s="87"/>
-      <c r="AU82" s="87"/>
-      <c r="AV82" s="87"/>
-      <c r="AW82" s="87"/>
-      <c r="AX82" s="87"/>
-      <c r="AY82" s="87"/>
-      <c r="AZ82" s="86"/>
-      <c r="BA82" s="87"/>
-      <c r="BB82" s="87"/>
-      <c r="BC82" s="87"/>
-      <c r="BD82" s="87"/>
-      <c r="BE82" s="87"/>
-      <c r="BF82" s="87"/>
-      <c r="BG82" s="87"/>
-      <c r="BH82" s="39"/>
-      <c r="BI82" s="35"/>
-      <c r="BJ82" s="35"/>
-      <c r="BK82" s="35"/>
-      <c r="BL82" s="35"/>
-      <c r="BM82" s="35"/>
-      <c r="BN82" s="35"/>
-      <c r="BO82" s="35"/>
-      <c r="BP82" s="34"/>
-      <c r="BQ82" s="44"/>
-      <c r="BR82" s="44"/>
-      <c r="BS82" s="44"/>
-      <c r="BT82" s="44"/>
-      <c r="BU82" s="44"/>
-      <c r="BV82" s="44"/>
-      <c r="BW82" s="44"/>
-      <c r="BX82" s="34"/>
-      <c r="BY82" s="44"/>
-      <c r="BZ82" s="44"/>
-      <c r="CA82" s="44"/>
-      <c r="CB82" s="44"/>
-      <c r="CC82" s="44"/>
-      <c r="CD82" s="44"/>
-      <c r="CE82" s="44"/>
-      <c r="CF82" s="86"/>
-      <c r="CG82" s="87"/>
-      <c r="CH82" s="87"/>
-      <c r="CI82" s="87"/>
-      <c r="CJ82" s="87"/>
-      <c r="CK82" s="87"/>
-      <c r="CL82" s="87"/>
-      <c r="CM82" s="87"/>
-      <c r="CN82" s="86"/>
-      <c r="CO82" s="87"/>
-      <c r="CP82" s="87"/>
-      <c r="CQ82" s="87"/>
-      <c r="CR82" s="87"/>
-      <c r="CS82" s="87"/>
-      <c r="CT82" s="87"/>
-      <c r="CU82" s="87"/>
-      <c r="CV82" s="86"/>
-      <c r="CW82" s="87"/>
-      <c r="CX82" s="87"/>
-      <c r="CY82" s="87"/>
-      <c r="CZ82" s="87"/>
-      <c r="DA82" s="87"/>
-      <c r="DB82" s="87"/>
-      <c r="DC82" s="87"/>
-      <c r="DD82" s="86"/>
-      <c r="DE82" s="87"/>
-      <c r="DF82" s="87"/>
-      <c r="DG82" s="87"/>
-      <c r="DH82" s="87"/>
-      <c r="DI82" s="87"/>
-      <c r="DJ82" s="87"/>
-      <c r="DK82" s="87"/>
-      <c r="DL82" s="34"/>
-      <c r="DM82" s="44"/>
-      <c r="DN82" s="44"/>
-      <c r="DO82" s="44"/>
-      <c r="DP82" s="44"/>
-      <c r="DQ82" s="44"/>
-      <c r="DR82" s="44"/>
-      <c r="DS82" s="44"/>
-      <c r="DT82" s="34"/>
-      <c r="DU82" s="44"/>
-      <c r="DV82" s="44"/>
-      <c r="DW82" s="44"/>
-      <c r="DX82" s="44"/>
-      <c r="DY82" s="44"/>
-      <c r="DZ82" s="44"/>
-      <c r="EA82" s="44"/>
-      <c r="EB82" s="34"/>
-      <c r="EC82" s="35"/>
-      <c r="ED82" s="44"/>
-      <c r="EE82" s="44"/>
-      <c r="EF82" s="44"/>
-      <c r="EG82" s="44"/>
-      <c r="EH82" s="44"/>
-      <c r="EI82" s="44"/>
-      <c r="EJ82" s="34"/>
-      <c r="EK82" s="35"/>
-      <c r="EL82" s="44"/>
-      <c r="EM82" s="44"/>
-      <c r="EN82" s="44"/>
-      <c r="EO82" s="44"/>
-      <c r="EP82" s="44"/>
-      <c r="EQ82" s="72"/>
-    </row>
-    <row r="83" spans="1:147" x14ac:dyDescent="0.25">
-      <c r="A83" s="16"/>
-      <c r="B83" s="55"/>
-      <c r="C83" s="9" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="D83" s="39"/>
-      <c r="E83" s="35"/>
-      <c r="F83" s="35"/>
-      <c r="G83" s="35"/>
-      <c r="H83" s="35"/>
-      <c r="I83" s="35"/>
-      <c r="J83" s="35"/>
-      <c r="K83" s="35"/>
-      <c r="L83" s="34"/>
-      <c r="M83" s="44"/>
-      <c r="N83" s="44"/>
-      <c r="O83" s="44"/>
-      <c r="P83" s="44"/>
-      <c r="Q83" s="44"/>
-      <c r="R83" s="44"/>
-      <c r="S83" s="44"/>
-      <c r="T83" s="34"/>
-      <c r="U83" s="44"/>
-      <c r="V83" s="44"/>
-      <c r="W83" s="44"/>
-      <c r="X83" s="44"/>
-      <c r="Y83" s="44"/>
-      <c r="Z83" s="44"/>
-      <c r="AA83" s="44"/>
-      <c r="AB83" s="34"/>
-      <c r="AC83" s="44"/>
-      <c r="AD83" s="44"/>
-      <c r="AE83" s="44"/>
-      <c r="AF83" s="44"/>
-      <c r="AG83" s="44"/>
-      <c r="AH83" s="44"/>
-      <c r="AI83" s="44"/>
-      <c r="AJ83" s="86"/>
-      <c r="AK83" s="87"/>
-      <c r="AL83" s="87"/>
-      <c r="AM83" s="87"/>
-      <c r="AN83" s="87"/>
-      <c r="AO83" s="87"/>
-      <c r="AP83" s="87"/>
-      <c r="AQ83" s="87"/>
-      <c r="AR83" s="86"/>
-      <c r="AS83" s="87"/>
-      <c r="AT83" s="87"/>
-      <c r="AU83" s="87"/>
-      <c r="AV83" s="87"/>
-      <c r="AW83" s="87"/>
-      <c r="AX83" s="87"/>
-      <c r="AY83" s="87"/>
-      <c r="AZ83" s="86"/>
-      <c r="BA83" s="87"/>
-      <c r="BB83" s="87"/>
-      <c r="BC83" s="87"/>
-      <c r="BD83" s="87"/>
-      <c r="BE83" s="87"/>
-      <c r="BF83" s="87"/>
-      <c r="BG83" s="87"/>
-      <c r="BH83" s="39"/>
-      <c r="BI83" s="35"/>
-      <c r="BJ83" s="35"/>
-      <c r="BK83" s="35"/>
-      <c r="BL83" s="35"/>
-      <c r="BM83" s="35"/>
-      <c r="BN83" s="35"/>
-      <c r="BO83" s="35"/>
-      <c r="BP83" s="34"/>
-      <c r="BQ83" s="44"/>
-      <c r="BR83" s="44"/>
-      <c r="BS83" s="44"/>
-      <c r="BT83" s="44"/>
-      <c r="BU83" s="44"/>
-      <c r="BV83" s="44"/>
-      <c r="BW83" s="44"/>
-      <c r="BX83" s="34"/>
-      <c r="BY83" s="44"/>
-      <c r="BZ83" s="44"/>
-      <c r="CA83" s="44"/>
-      <c r="CB83" s="44"/>
-      <c r="CC83" s="44"/>
-      <c r="CD83" s="44"/>
-      <c r="CE83" s="44"/>
-      <c r="CF83" s="86"/>
-      <c r="CG83" s="87"/>
-      <c r="CH83" s="87"/>
-      <c r="CI83" s="87"/>
-      <c r="CJ83" s="87"/>
-      <c r="CK83" s="87"/>
-      <c r="CL83" s="87"/>
-      <c r="CM83" s="87"/>
-      <c r="CN83" s="86"/>
-      <c r="CO83" s="87"/>
-      <c r="CP83" s="87"/>
-      <c r="CQ83" s="87"/>
-      <c r="CR83" s="87"/>
-      <c r="CS83" s="87"/>
-      <c r="CT83" s="87"/>
-      <c r="CU83" s="87"/>
-      <c r="CV83" s="86"/>
-      <c r="CW83" s="87"/>
-      <c r="CX83" s="87"/>
-      <c r="CY83" s="87"/>
-      <c r="CZ83" s="87"/>
-      <c r="DA83" s="87"/>
-      <c r="DB83" s="87"/>
-      <c r="DC83" s="87"/>
-      <c r="DD83" s="86"/>
-      <c r="DE83" s="87"/>
-      <c r="DF83" s="87"/>
-      <c r="DG83" s="87"/>
-      <c r="DH83" s="87"/>
-      <c r="DI83" s="87"/>
-      <c r="DJ83" s="87"/>
-      <c r="DK83" s="87"/>
-      <c r="DL83" s="34"/>
-      <c r="DM83" s="44"/>
-      <c r="DN83" s="44"/>
-      <c r="DO83" s="44"/>
-      <c r="DP83" s="44"/>
-      <c r="DQ83" s="44"/>
-      <c r="DR83" s="44"/>
-      <c r="DS83" s="44"/>
-      <c r="DT83" s="34"/>
-      <c r="DU83" s="44"/>
-      <c r="DV83" s="44"/>
-      <c r="DW83" s="44"/>
-      <c r="DX83" s="44"/>
-      <c r="DY83" s="44"/>
-      <c r="DZ83" s="44"/>
-      <c r="EA83" s="44"/>
-      <c r="EB83" s="34"/>
-      <c r="EC83" s="35"/>
-      <c r="ED83" s="44"/>
-      <c r="EE83" s="44"/>
-      <c r="EF83" s="44"/>
-      <c r="EG83" s="44"/>
-      <c r="EH83" s="44"/>
-      <c r="EI83" s="44"/>
-      <c r="EJ83" s="34"/>
-      <c r="EK83" s="35"/>
-      <c r="EL83" s="44"/>
-      <c r="EM83" s="44"/>
-      <c r="EN83" s="44"/>
-      <c r="EO83" s="44"/>
-      <c r="EP83" s="44"/>
-      <c r="EQ83" s="72"/>
-    </row>
-    <row r="84" spans="1:147" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="17"/>
-      <c r="B84" s="56"/>
-      <c r="C84" s="53" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="D84" s="40"/>
-      <c r="E84" s="37"/>
-      <c r="F84" s="37"/>
-      <c r="G84" s="37"/>
-      <c r="H84" s="37"/>
-      <c r="I84" s="37"/>
-      <c r="J84" s="37"/>
-      <c r="K84" s="37"/>
-      <c r="L84" s="36"/>
-      <c r="M84" s="45"/>
-      <c r="N84" s="45"/>
-      <c r="O84" s="45"/>
-      <c r="P84" s="45"/>
-      <c r="Q84" s="45"/>
-      <c r="R84" s="45"/>
-      <c r="S84" s="45"/>
-      <c r="T84" s="36"/>
-      <c r="U84" s="45"/>
-      <c r="V84" s="45"/>
-      <c r="W84" s="45"/>
-      <c r="X84" s="45"/>
-      <c r="Y84" s="45"/>
-      <c r="Z84" s="45"/>
-      <c r="AA84" s="45"/>
-      <c r="AB84" s="36"/>
-      <c r="AC84" s="45"/>
-      <c r="AD84" s="45"/>
-      <c r="AE84" s="45"/>
-      <c r="AF84" s="45"/>
-      <c r="AG84" s="45"/>
-      <c r="AH84" s="45"/>
-      <c r="AI84" s="45"/>
-      <c r="AJ84" s="88"/>
-      <c r="AK84" s="89"/>
-      <c r="AL84" s="89"/>
-      <c r="AM84" s="89"/>
-      <c r="AN84" s="89"/>
-      <c r="AO84" s="89"/>
-      <c r="AP84" s="89"/>
-      <c r="AQ84" s="89"/>
-      <c r="AR84" s="88"/>
-      <c r="AS84" s="89"/>
-      <c r="AT84" s="89"/>
-      <c r="AU84" s="89"/>
-      <c r="AV84" s="89"/>
-      <c r="AW84" s="89"/>
-      <c r="AX84" s="89"/>
-      <c r="AY84" s="89"/>
-      <c r="AZ84" s="88"/>
-      <c r="BA84" s="89"/>
-      <c r="BB84" s="89"/>
-      <c r="BC84" s="89"/>
-      <c r="BD84" s="89"/>
-      <c r="BE84" s="89"/>
-      <c r="BF84" s="89"/>
-      <c r="BG84" s="89"/>
-      <c r="BH84" s="40"/>
-      <c r="BI84" s="37"/>
-      <c r="BJ84" s="37"/>
-      <c r="BK84" s="37"/>
-      <c r="BL84" s="37"/>
-      <c r="BM84" s="37"/>
-      <c r="BN84" s="37"/>
-      <c r="BO84" s="37"/>
-      <c r="BP84" s="36"/>
-      <c r="BQ84" s="45"/>
-      <c r="BR84" s="45"/>
-      <c r="BS84" s="45"/>
-      <c r="BT84" s="45"/>
-      <c r="BU84" s="45"/>
-      <c r="BV84" s="45"/>
-      <c r="BW84" s="45"/>
-      <c r="BX84" s="36"/>
-      <c r="BY84" s="45"/>
-      <c r="BZ84" s="45"/>
-      <c r="CA84" s="45"/>
-      <c r="CB84" s="45"/>
-      <c r="CC84" s="45"/>
-      <c r="CD84" s="45"/>
-      <c r="CE84" s="45"/>
-      <c r="CF84" s="88"/>
-      <c r="CG84" s="89"/>
-      <c r="CH84" s="89"/>
-      <c r="CI84" s="89"/>
-      <c r="CJ84" s="89"/>
-      <c r="CK84" s="89"/>
-      <c r="CL84" s="89"/>
-      <c r="CM84" s="89"/>
-      <c r="CN84" s="88"/>
-      <c r="CO84" s="89"/>
-      <c r="CP84" s="89"/>
-      <c r="CQ84" s="89"/>
-      <c r="CR84" s="89"/>
-      <c r="CS84" s="89"/>
-      <c r="CT84" s="89"/>
-      <c r="CU84" s="89"/>
-      <c r="CV84" s="88"/>
-      <c r="CW84" s="89"/>
-      <c r="CX84" s="89"/>
-      <c r="CY84" s="89"/>
-      <c r="CZ84" s="89"/>
-      <c r="DA84" s="89"/>
-      <c r="DB84" s="89"/>
-      <c r="DC84" s="89"/>
-      <c r="DD84" s="88"/>
-      <c r="DE84" s="89"/>
-      <c r="DF84" s="89"/>
-      <c r="DG84" s="89"/>
-      <c r="DH84" s="89"/>
-      <c r="DI84" s="89"/>
-      <c r="DJ84" s="89"/>
-      <c r="DK84" s="89"/>
-      <c r="DL84" s="36"/>
-      <c r="DM84" s="45"/>
-      <c r="DN84" s="45"/>
-      <c r="DO84" s="45"/>
-      <c r="DP84" s="45"/>
-      <c r="DQ84" s="45"/>
-      <c r="DR84" s="45"/>
-      <c r="DS84" s="45"/>
-      <c r="DT84" s="36"/>
-      <c r="DU84" s="45"/>
-      <c r="DV84" s="45"/>
-      <c r="DW84" s="45"/>
-      <c r="DX84" s="45"/>
-      <c r="DY84" s="45"/>
-      <c r="DZ84" s="45"/>
-      <c r="EA84" s="45"/>
-      <c r="EB84" s="36"/>
-      <c r="EC84" s="37"/>
-      <c r="ED84" s="45"/>
-      <c r="EE84" s="45"/>
-      <c r="EF84" s="45"/>
-      <c r="EG84" s="45"/>
-      <c r="EH84" s="45"/>
-      <c r="EI84" s="45"/>
-      <c r="EJ84" s="36"/>
-      <c r="EK84" s="37"/>
-      <c r="EL84" s="45"/>
-      <c r="EM84" s="45"/>
-      <c r="EN84" s="45"/>
-      <c r="EO84" s="45"/>
-      <c r="EP84" s="45"/>
-      <c r="EQ84" s="73"/>
+      <c r="D82" s="40"/>
+      <c r="E82" s="37"/>
+      <c r="F82" s="37"/>
+      <c r="G82" s="37"/>
+      <c r="H82" s="37"/>
+      <c r="I82" s="37"/>
+      <c r="J82" s="37"/>
+      <c r="K82" s="37"/>
+      <c r="L82" s="36"/>
+      <c r="M82" s="45"/>
+      <c r="N82" s="45"/>
+      <c r="O82" s="45"/>
+      <c r="P82" s="45"/>
+      <c r="Q82" s="45"/>
+      <c r="R82" s="45"/>
+      <c r="S82" s="45"/>
+      <c r="T82" s="36"/>
+      <c r="U82" s="45"/>
+      <c r="V82" s="45"/>
+      <c r="W82" s="45"/>
+      <c r="X82" s="45"/>
+      <c r="Y82" s="45"/>
+      <c r="Z82" s="45"/>
+      <c r="AA82" s="45"/>
+      <c r="AB82" s="36"/>
+      <c r="AC82" s="45"/>
+      <c r="AD82" s="45"/>
+      <c r="AE82" s="45"/>
+      <c r="AF82" s="45"/>
+      <c r="AG82" s="45"/>
+      <c r="AH82" s="45"/>
+      <c r="AI82" s="45"/>
+      <c r="AJ82" s="88"/>
+      <c r="AK82" s="89"/>
+      <c r="AL82" s="89"/>
+      <c r="AM82" s="89"/>
+      <c r="AN82" s="89"/>
+      <c r="AO82" s="89"/>
+      <c r="AP82" s="89"/>
+      <c r="AQ82" s="89"/>
+      <c r="AR82" s="88"/>
+      <c r="AS82" s="89"/>
+      <c r="AT82" s="89"/>
+      <c r="AU82" s="89"/>
+      <c r="AV82" s="89"/>
+      <c r="AW82" s="89"/>
+      <c r="AX82" s="89"/>
+      <c r="AY82" s="89"/>
+      <c r="AZ82" s="88"/>
+      <c r="BA82" s="89"/>
+      <c r="BB82" s="89"/>
+      <c r="BC82" s="89"/>
+      <c r="BD82" s="89"/>
+      <c r="BE82" s="89"/>
+      <c r="BF82" s="89"/>
+      <c r="BG82" s="89"/>
+      <c r="BH82" s="40"/>
+      <c r="BI82" s="37"/>
+      <c r="BJ82" s="37"/>
+      <c r="BK82" s="37"/>
+      <c r="BL82" s="37"/>
+      <c r="BM82" s="37"/>
+      <c r="BN82" s="37"/>
+      <c r="BO82" s="37"/>
+      <c r="BP82" s="36"/>
+      <c r="BQ82" s="45"/>
+      <c r="BR82" s="45"/>
+      <c r="BS82" s="45"/>
+      <c r="BT82" s="45"/>
+      <c r="BU82" s="45"/>
+      <c r="BV82" s="45"/>
+      <c r="BW82" s="45"/>
+      <c r="BX82" s="36"/>
+      <c r="BY82" s="45"/>
+      <c r="BZ82" s="45"/>
+      <c r="CA82" s="45"/>
+      <c r="CB82" s="45"/>
+      <c r="CC82" s="45"/>
+      <c r="CD82" s="45"/>
+      <c r="CE82" s="45"/>
+      <c r="CF82" s="88"/>
+      <c r="CG82" s="89"/>
+      <c r="CH82" s="89"/>
+      <c r="CI82" s="89"/>
+      <c r="CJ82" s="89"/>
+      <c r="CK82" s="89"/>
+      <c r="CL82" s="89"/>
+      <c r="CM82" s="89"/>
+      <c r="CN82" s="88"/>
+      <c r="CO82" s="89"/>
+      <c r="CP82" s="89"/>
+      <c r="CQ82" s="89"/>
+      <c r="CR82" s="89"/>
+      <c r="CS82" s="89"/>
+      <c r="CT82" s="89"/>
+      <c r="CU82" s="89"/>
+      <c r="CV82" s="88"/>
+      <c r="CW82" s="89"/>
+      <c r="CX82" s="89"/>
+      <c r="CY82" s="89"/>
+      <c r="CZ82" s="89"/>
+      <c r="DA82" s="89"/>
+      <c r="DB82" s="89"/>
+      <c r="DC82" s="89"/>
+      <c r="DD82" s="88"/>
+      <c r="DE82" s="89"/>
+      <c r="DF82" s="89"/>
+      <c r="DG82" s="89"/>
+      <c r="DH82" s="89"/>
+      <c r="DI82" s="89"/>
+      <c r="DJ82" s="89"/>
+      <c r="DK82" s="89"/>
+      <c r="DL82" s="36"/>
+      <c r="DM82" s="45"/>
+      <c r="DN82" s="45"/>
+      <c r="DO82" s="45"/>
+      <c r="DP82" s="45"/>
+      <c r="DQ82" s="45"/>
+      <c r="DR82" s="45"/>
+      <c r="DS82" s="45"/>
+      <c r="DT82" s="36"/>
+      <c r="DU82" s="45"/>
+      <c r="DV82" s="45"/>
+      <c r="DW82" s="45"/>
+      <c r="DX82" s="45"/>
+      <c r="DY82" s="45"/>
+      <c r="DZ82" s="45"/>
+      <c r="EA82" s="45"/>
+      <c r="EB82" s="36"/>
+      <c r="EC82" s="37"/>
+      <c r="ED82" s="45"/>
+      <c r="EE82" s="45"/>
+      <c r="EF82" s="45"/>
+      <c r="EG82" s="45"/>
+      <c r="EH82" s="45"/>
+      <c r="EI82" s="45"/>
+      <c r="EJ82" s="36"/>
+      <c r="EK82" s="37"/>
+      <c r="EL82" s="45"/>
+      <c r="EM82" s="45"/>
+      <c r="EN82" s="45"/>
+      <c r="EO82" s="45"/>
+      <c r="EP82" s="45"/>
+      <c r="EQ82" s="73"/>
     </row>
   </sheetData>
   <sheetProtection insertRows="0"/>
   <mergeCells count="46">
-    <mergeCell ref="DD3:DK84"/>
-    <mergeCell ref="DD2:DK2"/>
     <mergeCell ref="DL2:DS2"/>
     <mergeCell ref="DT2:EA2"/>
     <mergeCell ref="EB2:EI2"/>
     <mergeCell ref="EJ2:EQ2"/>
     <mergeCell ref="A3:B3"/>
-    <mergeCell ref="AJ3:AQ84"/>
-    <mergeCell ref="AR3:AY84"/>
-    <mergeCell ref="AZ3:BG84"/>
-    <mergeCell ref="CF3:CM84"/>
+    <mergeCell ref="AJ3:AQ82"/>
+    <mergeCell ref="AR3:AY82"/>
+    <mergeCell ref="AZ3:BG82"/>
+    <mergeCell ref="CF3:CM82"/>
     <mergeCell ref="BH2:BO2"/>
     <mergeCell ref="BP2:BW2"/>
     <mergeCell ref="BX2:CE2"/>
     <mergeCell ref="CF2:CM2"/>
     <mergeCell ref="CN2:CU2"/>
     <mergeCell ref="CV2:DC2"/>
-    <mergeCell ref="CN3:CU84"/>
-    <mergeCell ref="CV3:DC84"/>
+    <mergeCell ref="CN3:CU82"/>
+    <mergeCell ref="CV3:DC82"/>
+    <mergeCell ref="DD3:DK82"/>
+    <mergeCell ref="DD2:DK2"/>
     <mergeCell ref="DT1:EA1"/>
     <mergeCell ref="EB1:EI1"/>
     <mergeCell ref="EJ1:EQ1"/>
@@ -30020,7 +29738,7 @@
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BH31:CE61 DL31:EQ61 D50:T52 X50:AI52 D31:AI49 D53:AI61 U52:W52">
+  <conditionalFormatting sqref="D48:T50 X48:AI50 D51:AI59 U50:W50 BH31:CE59 DL31:EQ59 D31:AI47">
     <cfRule type="cellIs" dxfId="63" priority="63" stopIfTrue="1" operator="equal">
       <formula>"R"</formula>
     </cfRule>
@@ -30028,7 +29746,7 @@
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D63:K72 T63:AA72 DL63:EI72 BH63:CE72">
+  <conditionalFormatting sqref="D61:K70 T61:AA70 DL61:EI70 BH61:CE70">
     <cfRule type="cellIs" dxfId="61" priority="61" stopIfTrue="1" operator="equal">
       <formula>"R"</formula>
     </cfRule>
@@ -30036,7 +29754,7 @@
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BH75:CE76 DL75:EI76 D75:K84 T75:AA84 BH78:CE84 DL78:EI84">
+  <conditionalFormatting sqref="BH73:CE74 DL73:EI74 D73:K82 T73:AA82 BH76:CE82 DL76:EI82">
     <cfRule type="cellIs" dxfId="59" priority="59" stopIfTrue="1" operator="equal">
       <formula>"R"</formula>
     </cfRule>
@@ -30052,7 +29770,7 @@
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L63:S63 L65:S72">
+  <conditionalFormatting sqref="L61:S61 L63:S70">
     <cfRule type="cellIs" dxfId="55" priority="55" stopIfTrue="1" operator="equal">
       <formula>"R"</formula>
     </cfRule>
@@ -30060,7 +29778,7 @@
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L75:S76 L78:S84">
+  <conditionalFormatting sqref="L73:S74 L76:S82">
     <cfRule type="cellIs" dxfId="53" priority="53" stopIfTrue="1" operator="equal">
       <formula>"R"</formula>
     </cfRule>
@@ -30076,7 +29794,7 @@
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AB63:AI63 AB65:AI72">
+  <conditionalFormatting sqref="AB61:AI61 AB63:AI70">
     <cfRule type="cellIs" dxfId="49" priority="49" stopIfTrue="1" operator="equal">
       <formula>"R"</formula>
     </cfRule>
@@ -30084,7 +29802,7 @@
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AB75:AI76 AB78:AI84">
+  <conditionalFormatting sqref="AB73:AI74 AB76:AI82">
     <cfRule type="cellIs" dxfId="47" priority="47" stopIfTrue="1" operator="equal">
       <formula>"R"</formula>
     </cfRule>
@@ -30108,7 +29826,7 @@
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="EJ63:EQ63 EJ66:EQ72">
+  <conditionalFormatting sqref="EJ61:EQ61 EJ64:EQ70">
     <cfRule type="cellIs" dxfId="41" priority="41" stopIfTrue="1" operator="equal">
       <formula>"R"</formula>
     </cfRule>
@@ -30116,7 +29834,7 @@
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="EJ78:EQ84">
+  <conditionalFormatting sqref="EJ76:EQ82">
     <cfRule type="cellIs" dxfId="39" priority="39" stopIfTrue="1" operator="equal">
       <formula>"R"</formula>
     </cfRule>
@@ -30124,7 +29842,7 @@
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L64:S64">
+  <conditionalFormatting sqref="L62:S62">
     <cfRule type="cellIs" dxfId="37" priority="37" stopIfTrue="1" operator="equal">
       <formula>"R"</formula>
     </cfRule>
@@ -30132,7 +29850,7 @@
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AB64:AI64">
+  <conditionalFormatting sqref="AB62:AI62">
     <cfRule type="cellIs" dxfId="35" priority="35" stopIfTrue="1" operator="equal">
       <formula>"R"</formula>
     </cfRule>
@@ -30140,7 +29858,7 @@
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="EJ64:EP64">
+  <conditionalFormatting sqref="EJ62:EP62">
     <cfRule type="cellIs" dxfId="33" priority="33" stopIfTrue="1" operator="equal">
       <formula>"R"</formula>
     </cfRule>
@@ -30148,7 +29866,7 @@
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U50:W51">
+  <conditionalFormatting sqref="U48:W49">
     <cfRule type="cellIs" dxfId="31" priority="31" stopIfTrue="1" operator="equal">
       <formula>"R"</formula>
     </cfRule>
@@ -30164,7 +29882,7 @@
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="EQ64">
+  <conditionalFormatting sqref="EQ62">
     <cfRule type="cellIs" dxfId="27" priority="25" stopIfTrue="1" operator="equal">
       <formula>"R"</formula>
     </cfRule>
@@ -30172,7 +29890,7 @@
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="EJ65:EQ65">
+  <conditionalFormatting sqref="EJ63:EQ63">
     <cfRule type="cellIs" dxfId="25" priority="27" stopIfTrue="1" operator="equal">
       <formula>"R"</formula>
     </cfRule>
@@ -30180,7 +29898,7 @@
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L77:S77">
+  <conditionalFormatting sqref="L75:S75">
     <cfRule type="cellIs" dxfId="23" priority="23" stopIfTrue="1" operator="equal">
       <formula>"R"</formula>
     </cfRule>
@@ -30188,7 +29906,7 @@
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="EJ77:EQ77">
+  <conditionalFormatting sqref="EJ75:EQ75">
     <cfRule type="cellIs" dxfId="21" priority="7" stopIfTrue="1" operator="equal">
       <formula>"R"</formula>
     </cfRule>
@@ -30196,7 +29914,7 @@
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AB77:AI77">
+  <conditionalFormatting sqref="AB75:AI75">
     <cfRule type="cellIs" dxfId="19" priority="21" stopIfTrue="1" operator="equal">
       <formula>"R"</formula>
     </cfRule>
@@ -30204,7 +29922,7 @@
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BH77:BO77">
+  <conditionalFormatting sqref="BH75:BO75">
     <cfRule type="cellIs" dxfId="17" priority="19" stopIfTrue="1" operator="equal">
       <formula>"R"</formula>
     </cfRule>
@@ -30212,7 +29930,7 @@
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BP77:BW77">
+  <conditionalFormatting sqref="BP75:BW75">
     <cfRule type="cellIs" dxfId="15" priority="17" stopIfTrue="1" operator="equal">
       <formula>"R"</formula>
     </cfRule>
@@ -30220,7 +29938,7 @@
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BX77:CE77">
+  <conditionalFormatting sqref="BX75:CE75">
     <cfRule type="cellIs" dxfId="13" priority="15" stopIfTrue="1" operator="equal">
       <formula>"R"</formula>
     </cfRule>
@@ -30228,7 +29946,7 @@
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="DL77:DS77">
+  <conditionalFormatting sqref="DL75:DS75">
     <cfRule type="cellIs" dxfId="11" priority="13" stopIfTrue="1" operator="equal">
       <formula>"R"</formula>
     </cfRule>
@@ -30236,7 +29954,7 @@
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="DT77:EA77">
+  <conditionalFormatting sqref="DT75:EA75">
     <cfRule type="cellIs" dxfId="9" priority="11" stopIfTrue="1" operator="equal">
       <formula>"R"</formula>
     </cfRule>
@@ -30244,7 +29962,7 @@
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="EB77:EI77">
+  <conditionalFormatting sqref="EB75:EI75">
     <cfRule type="cellIs" dxfId="7" priority="9" stopIfTrue="1" operator="equal">
       <formula>"R"</formula>
     </cfRule>
@@ -30252,7 +29970,7 @@
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="EJ74:EQ74">
+  <conditionalFormatting sqref="EJ72:EQ72">
     <cfRule type="cellIs" dxfId="5" priority="1" stopIfTrue="1" operator="equal">
       <formula>"R"</formula>
     </cfRule>
@@ -30260,7 +29978,7 @@
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="EB74:EI74">
+  <conditionalFormatting sqref="EB72:EI72">
     <cfRule type="cellIs" dxfId="3" priority="5" stopIfTrue="1" operator="equal">
       <formula>"R"</formula>
     </cfRule>
@@ -30268,7 +29986,7 @@
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="EJ75:EQ76">
+  <conditionalFormatting sqref="EJ73:EQ74">
     <cfRule type="cellIs" dxfId="1" priority="3" stopIfTrue="1" operator="equal">
       <formula>"R"</formula>
     </cfRule>

</xml_diff>